<commit_message>
Update questions-data.js from Excel - 496 hyperlinks
- Regenerated from Self Assessment Structure - Master.xlsx
- Updated Resources and Tools links as per user edits
- 113 questions, 496 total hyperlinks

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Self Assessment Structure - Master.xlsx
+++ b/Self Assessment Structure - Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\janek\sova-mvp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CBDD62-A83D-40AC-B0E2-6998E801EFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FDDEB-4C52-4A28-B414-B28D0DDD9CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5690,12 +5690,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6253,7 +6253,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>1348</v>
       </c>
       <c r="B2" s="34"/>
@@ -6373,7 +6373,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="35" t="s">
         <v>1375</v>
       </c>
       <c r="B11" s="34"/>
@@ -6479,7 +6479,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="35" t="s">
         <v>1404</v>
       </c>
       <c r="B19" s="34"/>
@@ -6571,7 +6571,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="35" t="s">
         <v>1429</v>
       </c>
       <c r="B26" s="34"/>
@@ -6775,7 +6775,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="35" t="s">
         <v>1486</v>
       </c>
       <c r="B41" s="34"/>
@@ -6853,7 +6853,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="35" t="s">
         <v>1507</v>
       </c>
       <c r="B47" s="34"/>
@@ -7113,7 +7113,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="35" t="s">
         <v>1578</v>
       </c>
       <c r="B66" s="34"/>
@@ -7121,7 +7121,7 @@
       <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="33" t="s">
         <v>1579</v>
       </c>
       <c r="B67" s="34"/>
@@ -7227,7 +7227,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="33" t="s">
         <v>1607</v>
       </c>
       <c r="B75" s="34"/>
@@ -7277,7 +7277,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="35" t="s">
+      <c r="A79" s="33" t="s">
         <v>1620</v>
       </c>
       <c r="B79" s="34"/>
@@ -7299,7 +7299,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="35" t="s">
+      <c r="A81" s="33" t="s">
         <v>1625</v>
       </c>
       <c r="B81" s="34"/>
@@ -7321,7 +7321,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="35" t="s">
+      <c r="A83" s="33" t="s">
         <v>1630</v>
       </c>
       <c r="B83" s="34"/>
@@ -7358,6 +7358,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A66:D66"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="A79:D79"/>
@@ -7365,11 +7370,6 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7946,10 +7946,10 @@
   <dimension ref="A1:U117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13115,501 +13115,501 @@
   <phoneticPr fontId="20" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="I2" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="P2" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="R2" r:id="rId6" display="&quot;Governance Problems - Lack of foundational legal structure, compliance oversight, and board governance creates operational vulnerability and limits investment readiness&quot;" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="G3" r:id="rId7" display="Shareholders Agreement Template (if Team)" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="P3" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="R3" r:id="rId9" display="&quot;Shareholder Disagreement - Differences of opinion among founders create disputes when foundational strategy and conflict resolution aren't established&quot;" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="G4" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="H4" r:id="rId11" display="Brene Brown - Dare to Lead" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="J4" r:id="rId12" display="Core Values Definition Workshop" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="P4" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="R4" r:id="rId14" display="Don’t attempt the entrepreneurial journey solo. Numerous startups fail because they lack a robust network of supporters who can help promote their business. This includes organisations embarking on similar ventures, suppliers who can cater to startup needs, and industry veterans who have already achieved success. " xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="S4" r:id="rId15" display="Don’t attempt the entrepreneurial journey solo. Numerous startups fail because they lack a robust network of supporters who can help promote their business. This includes organisations embarking on similar ventures, suppliers who can cater to startup needs, and industry veterans who have already achieved success. " xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="T4" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
-    <hyperlink ref="I5" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
-    <hyperlink ref="J5" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
-    <hyperlink ref="K5" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
-    <hyperlink ref="L5" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
-    <hyperlink ref="N5" r:id="rId21" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
-    <hyperlink ref="P5" r:id="rId22" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
-    <hyperlink ref="R5" r:id="rId23" display="In retrospect, 51.3% of the surveyed founders thought they were adequately prepared when they launched their startup. No wonder so many advised better planning. “Research, research, research. Research your market,” said one founder. To that we offer an addendum: turn all that research into a business plan." xr:uid="{00000000-0004-0000-0500-000016000000}"/>
-    <hyperlink ref="T5" r:id="rId24" display="suppose the startup owner fails to draw up a comprehensive business plan or build a business model that seems sustainable over the long run. In that case, the startup might lose money, encounter operational issues, and run into legal problems." xr:uid="{00000000-0004-0000-0500-000017000000}"/>
-    <hyperlink ref="U5" r:id="rId25" xr:uid="{00000000-0004-0000-0500-000018000000}"/>
-    <hyperlink ref="H6" r:id="rId26" xr:uid="{00000000-0004-0000-0500-000019000000}"/>
-    <hyperlink ref="I6" r:id="rId27" xr:uid="{00000000-0004-0000-0500-00001A000000}"/>
-    <hyperlink ref="J6" r:id="rId28" display="Jobs To Be Done Framework" xr:uid="{00000000-0004-0000-0500-00001B000000}"/>
-    <hyperlink ref="K6" r:id="rId29" xr:uid="{00000000-0004-0000-0500-00001C000000}"/>
-    <hyperlink ref="P6" r:id="rId30" xr:uid="{00000000-0004-0000-0500-00001D000000}"/>
-    <hyperlink ref="R6" r:id="rId31" display="&quot;Overwhelming Competition - Inability to keep pace with innovators or differentiate&quot;" xr:uid="{00000000-0004-0000-0500-00001E000000}"/>
-    <hyperlink ref="S6" r:id="rId32" display="Emulation may be the sincerest form of flattery, but it does not always translate into good business. Understanding the existing market players is critical if you intend to capitalise on being a fast follower. However, it’s important to note that many start-ups that merely follow trends often fail." xr:uid="{00000000-0004-0000-0500-00001F000000}"/>
-    <hyperlink ref="G7" r:id="rId33" xr:uid="{00000000-0004-0000-0500-000020000000}"/>
-    <hyperlink ref="H7" r:id="rId34" xr:uid="{00000000-0004-0000-0500-000021000000}"/>
-    <hyperlink ref="I7" r:id="rId35" xr:uid="{00000000-0004-0000-0500-000022000000}"/>
-    <hyperlink ref="P7" r:id="rId36" xr:uid="{00000000-0004-0000-0500-000023000000}"/>
-    <hyperlink ref="R7" r:id="rId37" display="&quot;Poor Tax and Statutory Compliance - Missing taxes, superannuation, and insurance obligations damages creditworthiness and business value&quot;" xr:uid="{00000000-0004-0000-0500-000024000000}"/>
-    <hyperlink ref="G8" r:id="rId38" xr:uid="{00000000-0004-0000-0500-000025000000}"/>
-    <hyperlink ref="H8" r:id="rId39" xr:uid="{00000000-0004-0000-0500-000026000000}"/>
-    <hyperlink ref="I8" r:id="rId40" xr:uid="{00000000-0004-0000-0500-000027000000}"/>
-    <hyperlink ref="P8" r:id="rId41" display="Proof of Concept and Validation are significant factors that VCs consider when assessing startups. VCs want to see evidence that the startup's product or service has been tested or proven in the market. This validation shows that there is demand for the offering and reduces the risk of failure. It can be demonstrated through metrics such as user adoption, revenue growth, or partnerships." xr:uid="{00000000-0004-0000-0500-000028000000}"/>
-    <hyperlink ref="R8" r:id="rId42" display="Startups waste months building features nobody wants. An MVP should test your riskiest assumption with minimum effort. - Ash Maurya" xr:uid="{00000000-0004-0000-0500-000029000000}"/>
-    <hyperlink ref="I9" r:id="rId43" xr:uid="{00000000-0004-0000-0500-00002A000000}"/>
-    <hyperlink ref="J9" r:id="rId44" xr:uid="{00000000-0004-0000-0500-00002B000000}"/>
-    <hyperlink ref="N9" r:id="rId45" xr:uid="{00000000-0004-0000-0500-00002D000000}"/>
-    <hyperlink ref="P9" r:id="rId46" xr:uid="{00000000-0004-0000-0500-00002E000000}"/>
-    <hyperlink ref="R9" r:id="rId47" xr:uid="{00000000-0004-0000-0500-00002F000000}"/>
-    <hyperlink ref="S9" r:id="rId48" display=" if no market exists for the startup’s product or service, even the most creative and well-executed marketing strategy will fail. Extensive market research is crucial to ensure that there is a product-market fit." xr:uid="{00000000-0004-0000-0500-000030000000}"/>
-    <hyperlink ref="L10" r:id="rId49" xr:uid="{00000000-0004-0000-0500-000031000000}"/>
-    <hyperlink ref="P10" r:id="rId50" xr:uid="{00000000-0004-0000-0500-000034000000}"/>
-    <hyperlink ref="R10" r:id="rId51" display="&quot;Focusing on Marketing Too Little or Too Late - Underinvesting in strategic marketing or depending on single channels, limiting scalability and creating vulnerability&quot;" xr:uid="{00000000-0004-0000-0500-000035000000}"/>
-    <hyperlink ref="S10" r:id="rId52" display="&quot;Neglecting Marketing and Sales - 14% of startups fail because of poor marketing efforts — founders focus on product while ignoring customer acquisition&quot;" xr:uid="{00000000-0004-0000-0500-000036000000}"/>
-    <hyperlink ref="O11" r:id="rId53" display="Yet by neglecting to research customer needs before commencing their engineering efforts, entrepreneurs end up wasting valuable time and capital on MVPs that are likely to miss their mark. These are false starts." xr:uid="{00000000-0004-0000-0500-000037000000}"/>
-    <hyperlink ref="P11" r:id="rId54" xr:uid="{00000000-0004-0000-0500-000038000000}"/>
-    <hyperlink ref="R11" r:id="rId55" xr:uid="{00000000-0004-0000-0500-000039000000}"/>
-    <hyperlink ref="S11" r:id="rId56" xr:uid="{00000000-0004-0000-0500-00003A000000}"/>
-    <hyperlink ref="T11" r:id="rId57" xr:uid="{00000000-0004-0000-0500-00003B000000}"/>
-    <hyperlink ref="P12" r:id="rId58" xr:uid="{00000000-0004-0000-0500-00003C000000}"/>
-    <hyperlink ref="R12" r:id="rId59" xr:uid="{00000000-0004-0000-0500-00003D000000}"/>
-    <hyperlink ref="S12" r:id="rId60" xr:uid="{00000000-0004-0000-0500-00003E000000}"/>
-    <hyperlink ref="T12" r:id="rId61" xr:uid="{00000000-0004-0000-0500-00003F000000}"/>
-    <hyperlink ref="U12" r:id="rId62" xr:uid="{00000000-0004-0000-0500-000040000000}"/>
-    <hyperlink ref="P13" r:id="rId63" xr:uid="{00000000-0004-0000-0500-000041000000}"/>
-    <hyperlink ref="R13" r:id="rId64" xr:uid="{00000000-0004-0000-0500-000042000000}"/>
-    <hyperlink ref="T13" r:id="rId65" xr:uid="{00000000-0004-0000-0500-000043000000}"/>
-    <hyperlink ref="U13" r:id="rId66" xr:uid="{00000000-0004-0000-0500-000044000000}"/>
-    <hyperlink ref="O14" r:id="rId67" xr:uid="{00000000-0004-0000-0500-000045000000}"/>
-    <hyperlink ref="P14" r:id="rId68" xr:uid="{00000000-0004-0000-0500-000046000000}"/>
-    <hyperlink ref="R14" r:id="rId69" xr:uid="{00000000-0004-0000-0500-000047000000}"/>
-    <hyperlink ref="S14" r:id="rId70" xr:uid="{00000000-0004-0000-0500-000048000000}"/>
-    <hyperlink ref="T14" r:id="rId71" display="Obsess over cash flow projections and monitor burn rate. Start small and scale slowly in conjunction with validated customer demand. Consider starting a side hustle income stream to self-fund your startup." xr:uid="{00000000-0004-0000-0500-000049000000}"/>
-    <hyperlink ref="P15" r:id="rId72" xr:uid="{00000000-0004-0000-0500-00004A000000}"/>
-    <hyperlink ref="R15" r:id="rId73" xr:uid="{00000000-0004-0000-0500-00004B000000}"/>
-    <hyperlink ref="S15" r:id="rId74" xr:uid="{00000000-0004-0000-0500-00004C000000}"/>
-    <hyperlink ref="P16" r:id="rId75" xr:uid="{00000000-0004-0000-0500-00004D000000}"/>
-    <hyperlink ref="R16" r:id="rId76" display="While some mistakes can be attributed to sheer bad luck or external factors, most of them are caused by repeated errors on the part of the business owner. Failing to recognize patterns in one's missteps and make the needed adjustments can lead to a lack of growth or even closure." xr:uid="{00000000-0004-0000-0500-00004E000000}"/>
-    <hyperlink ref="P17" r:id="rId77" xr:uid="{00000000-0004-0000-0500-00004F000000}"/>
-    <hyperlink ref="P18" r:id="rId78" xr:uid="{00000000-0004-0000-0500-000050000000}"/>
-    <hyperlink ref="R18" r:id="rId79" xr:uid="{00000000-0004-0000-0500-000051000000}"/>
-    <hyperlink ref="S18" r:id="rId80" xr:uid="{00000000-0004-0000-0500-000052000000}"/>
-    <hyperlink ref="T18" r:id="rId81" xr:uid="{00000000-0004-0000-0500-000053000000}"/>
-    <hyperlink ref="P19" r:id="rId82" xr:uid="{00000000-0004-0000-0500-000054000000}"/>
-    <hyperlink ref="R19" r:id="rId83" display="Unforeseen situations occur, market trends change and aggressive competitors can pop up out of nowhere. Consequently, you may need to change course quickly at one point or another." xr:uid="{00000000-0004-0000-0500-000055000000}"/>
-    <hyperlink ref="S19" r:id="rId84" xr:uid="{00000000-0004-0000-0500-000056000000}"/>
-    <hyperlink ref="T19" r:id="rId85" xr:uid="{00000000-0004-0000-0500-000057000000}"/>
-    <hyperlink ref="P20" r:id="rId86" xr:uid="{00000000-0004-0000-0500-000058000000}"/>
-    <hyperlink ref="R20" r:id="rId87" display="Human capital is essential for startups to scale effectively and efficiently. Having the right people at the right time can greatly enhance a startup’s ability to navigate the complexities of expanding markets, evolving customer demands, and increasingly intricate operations." xr:uid="{00000000-0004-0000-0500-000059000000}"/>
-    <hyperlink ref="P21" r:id="rId88" xr:uid="{00000000-0004-0000-0500-00005A000000}"/>
-    <hyperlink ref="P22" r:id="rId89" xr:uid="{00000000-0004-0000-0500-00005B000000}"/>
-    <hyperlink ref="O23" r:id="rId90" xr:uid="{00000000-0004-0000-0500-00005C000000}"/>
-    <hyperlink ref="P23" r:id="rId91" xr:uid="{00000000-0004-0000-0500-00005D000000}"/>
-    <hyperlink ref="T23" r:id="rId92" xr:uid="{00000000-0004-0000-0500-00005E000000}"/>
-    <hyperlink ref="P24" r:id="rId93" xr:uid="{00000000-0004-0000-0500-00005F000000}"/>
-    <hyperlink ref="T24" r:id="rId94" xr:uid="{00000000-0004-0000-0500-000060000000}"/>
-    <hyperlink ref="O25" r:id="rId95" xr:uid="{00000000-0004-0000-0500-000061000000}"/>
-    <hyperlink ref="P25" r:id="rId96" xr:uid="{00000000-0004-0000-0500-000062000000}"/>
-    <hyperlink ref="R25" r:id="rId97" xr:uid="{00000000-0004-0000-0500-000063000000}"/>
-    <hyperlink ref="P26" r:id="rId98" xr:uid="{00000000-0004-0000-0500-000064000000}"/>
-    <hyperlink ref="R26" r:id="rId99" xr:uid="{00000000-0004-0000-0500-000065000000}"/>
-    <hyperlink ref="S26" r:id="rId100" xr:uid="{00000000-0004-0000-0500-000066000000}"/>
-    <hyperlink ref="G27" r:id="rId101" xr:uid="{00000000-0004-0000-0500-000067000000}"/>
-    <hyperlink ref="H27" r:id="rId102" display="RACI Matrix" xr:uid="{00000000-0004-0000-0500-000068000000}"/>
-    <hyperlink ref="I27" r:id="rId103" display="RAPID Decision Framework" xr:uid="{00000000-0004-0000-0500-000069000000}"/>
-    <hyperlink ref="P27" r:id="rId104" xr:uid="{00000000-0004-0000-0500-00006A000000}"/>
-    <hyperlink ref="R27" r:id="rId105" display="&quot;Misaligned Co-Founder Expectations - Unspoken assumptions create partnership breakdown. 24% of co-founder relationships dissolve within four years&quot;" xr:uid="{00000000-0004-0000-0500-00006B000000}"/>
-    <hyperlink ref="S27" r:id="rId106" display="As Dima Maslennikov notes in his recent Entrepreneur.com article on co-founder alignment, misaligned expectations and unspoken assumptions are among the top reasons partnerships break down. His research shows that 24% of co-founder relationships dissolve within four years, often because initial commitment levels were mismatched from day one." xr:uid="{00000000-0004-0000-0500-00006C000000}"/>
-    <hyperlink ref="F28" r:id="rId107" xr:uid="{00000000-0004-0000-0500-00006D000000}"/>
-    <hyperlink ref="H28" r:id="rId108" xr:uid="{00000000-0004-0000-0500-00006E000000}"/>
-    <hyperlink ref="J28" r:id="rId109" xr:uid="{00000000-0004-0000-0500-00006F000000}"/>
-    <hyperlink ref="P28" r:id="rId110" xr:uid="{00000000-0004-0000-0500-000070000000}"/>
-    <hyperlink ref="R28" r:id="rId111" xr:uid="{00000000-0004-0000-0500-000071000000}"/>
-    <hyperlink ref="S28" r:id="rId112" display="&quot;Missing taxes, superannuation, and insurance obligations damages creditworthiness and business value&quot;" xr:uid="{00000000-0004-0000-0500-000072000000}"/>
-    <hyperlink ref="G29" r:id="rId113" xr:uid="{00000000-0004-0000-0500-000073000000}"/>
-    <hyperlink ref="H29" r:id="rId114" xr:uid="{00000000-0004-0000-0500-000074000000}"/>
-    <hyperlink ref="I29" r:id="rId115" xr:uid="{00000000-0004-0000-0500-000075000000}"/>
-    <hyperlink ref="J29" r:id="rId116" xr:uid="{00000000-0004-0000-0500-000076000000}"/>
-    <hyperlink ref="O29" r:id="rId117" xr:uid="{00000000-0004-0000-0500-000077000000}"/>
-    <hyperlink ref="P29" r:id="rId118" xr:uid="{00000000-0004-0000-0500-000078000000}"/>
-    <hyperlink ref="R29" r:id="rId119" display="&quot;Creating vs Satisfying Demand - It's easier to satisfy an existing need than create demand; realistic projections of target audience are essential&quot;" xr:uid="{00000000-0004-0000-0500-000079000000}"/>
-    <hyperlink ref="S29" r:id="rId120" display="&quot;False Positives - Founders misinterpret early adopter enthusiasm as mainstream demand, then discover later customers have different needs&quot;" xr:uid="{00000000-0004-0000-0500-00007A000000}"/>
-    <hyperlink ref="T29" r:id="rId121" display="you should regularly assess how your startup solves customer problems and determine whether your pricing adequately covers any costs associated with providing a service or product." xr:uid="{00000000-0004-0000-0500-00007B000000}"/>
-    <hyperlink ref="G30" r:id="rId122" xr:uid="{00000000-0004-0000-0500-00007C000000}"/>
-    <hyperlink ref="H30" r:id="rId123" xr:uid="{00000000-0004-0000-0500-00007D000000}"/>
-    <hyperlink ref="I30" r:id="rId124" xr:uid="{00000000-0004-0000-0500-00007E000000}"/>
-    <hyperlink ref="P30" r:id="rId125" xr:uid="{00000000-0004-0000-0500-00007F000000}"/>
-    <hyperlink ref="R30" r:id="rId126" display="&quot;Marketing Problems (56%) - Lack of product-market fit; insufficient validation of assumptions before resource investment. Don't invest a lot of time and resources before you are confident people want what you are offering.&quot;" xr:uid="{00000000-0004-0000-0500-000080000000}"/>
-    <hyperlink ref="S30" r:id="rId127" display="Early-stage startups need to spend up to 3x longer validating their target markets than their founders anticipate. One of the aims of the more extended market validation period is to prevent cash flow issues from running the project into the ground before the startup has the chance to determine the market-product fit." xr:uid="{00000000-0004-0000-0500-000081000000}"/>
-    <hyperlink ref="T30" r:id="rId128" xr:uid="{00000000-0004-0000-0500-000082000000}"/>
-    <hyperlink ref="H31" r:id="rId129" xr:uid="{00000000-0004-0000-0500-000084000000}"/>
-    <hyperlink ref="R31" r:id="rId130" display="&quot;Competitive Blindness - Entrepreneurs who skip competitive analysis and user testing of rival products miss critical insights about market strengths and weaknesses&quot;" xr:uid="{00000000-0004-0000-0500-000087000000}"/>
-    <hyperlink ref="G31" r:id="rId131" xr:uid="{00000000-0004-0000-0500-000089000000}"/>
-    <hyperlink ref="J31" r:id="rId132" xr:uid="{00000000-0004-0000-0500-00008A000000}"/>
-    <hyperlink ref="P31" r:id="rId133" xr:uid="{00000000-0004-0000-0500-00008B000000}"/>
-    <hyperlink ref="S31" r:id="rId134" display="&quot;42% of startups fail from no market need. Surveys lie - people say they'll buy, then don't. Test with behaviour (pre-orders, pilots), not surveys.&quot; - CB Insights" xr:uid="{00000000-0004-0000-0500-00008C000000}"/>
-    <hyperlink ref="T31" r:id="rId135" display="Conducting market surveys, engaging with potential customers, identifying competitors, and exploring untapped market opportunities are essential. These actions significantly reduce the risk of a startup’s efforts being in vain, ensuring a more informed and strategic approach to market entry. " xr:uid="{00000000-0004-0000-0500-00008D000000}"/>
-    <hyperlink ref="U31" r:id="rId136" xr:uid="{00000000-0004-0000-0500-00008E000000}"/>
-    <hyperlink ref="G32" r:id="rId137" xr:uid="{00000000-0004-0000-0500-00008F000000}"/>
-    <hyperlink ref="H32" r:id="rId138" xr:uid="{00000000-0004-0000-0500-000090000000}"/>
-    <hyperlink ref="N32" r:id="rId139" xr:uid="{00000000-0004-0000-0500-000091000000}"/>
-    <hyperlink ref="U32" r:id="rId140" location=":~:text=changes%20can%20reveal%20surprising%20and,you%20might've%20never%20expected.&amp;text=Even%20the%20best%20qualitative%20theory,a%20greater%20height%20through%20experimentation." xr:uid="{00000000-0004-0000-0500-000093000000}"/>
-    <hyperlink ref="G33" r:id="rId141" xr:uid="{00000000-0004-0000-0500-000094000000}"/>
-    <hyperlink ref="H33" r:id="rId142" xr:uid="{00000000-0004-0000-0500-000095000000}"/>
-    <hyperlink ref="I33" r:id="rId143" xr:uid="{00000000-0004-0000-0500-000096000000}"/>
-    <hyperlink ref="J33" r:id="rId144" xr:uid="{00000000-0004-0000-0500-000097000000}"/>
-    <hyperlink ref="N33" r:id="rId145" xr:uid="{00000000-0004-0000-0500-000098000000}"/>
-    <hyperlink ref="P33" r:id="rId146" xr:uid="{00000000-0004-0000-0500-000099000000}"/>
-    <hyperlink ref="R33" r:id="rId147" xr:uid="{00000000-0004-0000-0500-00009A000000}"/>
-    <hyperlink ref="T33" r:id="rId148" xr:uid="{00000000-0004-0000-0500-00009B000000}"/>
-    <hyperlink ref="U33" r:id="rId149" xr:uid="{00000000-0004-0000-0500-00009C000000}"/>
-    <hyperlink ref="G34" r:id="rId150" xr:uid="{00000000-0004-0000-0500-00009D000000}"/>
-    <hyperlink ref="H34" r:id="rId151" xr:uid="{00000000-0004-0000-0500-00009E000000}"/>
-    <hyperlink ref="I34" r:id="rId152" display="Pilot Program Framework" xr:uid="{00000000-0004-0000-0500-00009F000000}"/>
-    <hyperlink ref="P34" r:id="rId153" xr:uid="{00000000-0004-0000-0500-0000A0000000}"/>
-    <hyperlink ref="R34" r:id="rId154" display="&quot;Research-Free Launch - Launching without thorough market research is a recipe for financial loss; demand validation is crucial before investment&quot;" xr:uid="{00000000-0004-0000-0500-0000A1000000}"/>
-    <hyperlink ref="G35" r:id="rId155" xr:uid="{00000000-0004-0000-0500-0000A2000000}"/>
-    <hyperlink ref="H35" r:id="rId156" xr:uid="{00000000-0004-0000-0500-0000A3000000}"/>
-    <hyperlink ref="I35" r:id="rId157" display="Activation Metric Examples" xr:uid="{00000000-0004-0000-0500-0000A4000000}"/>
-    <hyperlink ref="J35" r:id="rId158" xr:uid="{00000000-0004-0000-0500-0000A5000000}"/>
-    <hyperlink ref="P35" r:id="rId159" xr:uid="{00000000-0004-0000-0500-0000A6000000}"/>
-    <hyperlink ref="R35" r:id="rId160" xr:uid="{00000000-0004-0000-0500-0000A7000000}"/>
-    <hyperlink ref="T35" r:id="rId161" display="&quot;DAU/MAU ratio of 20%+ is good for most consumer products. If it's dropping, you have an engagement problem before you have a growth problem.&quot; - Lenny Rachitsky" xr:uid="{00000000-0004-0000-0500-0000A8000000}"/>
-    <hyperlink ref="G36" r:id="rId162" display="Pre-Launch Marketing Tactics" xr:uid="{00000000-0004-0000-0500-0000A9000000}"/>
-    <hyperlink ref="H36" r:id="rId163" xr:uid="{00000000-0004-0000-0500-0000AA000000}"/>
-    <hyperlink ref="I36" r:id="rId164" xr:uid="{00000000-0004-0000-0500-0000AB000000}"/>
-    <hyperlink ref="P36" r:id="rId165" xr:uid="{00000000-0004-0000-0500-0000AC000000}"/>
-    <hyperlink ref="R36" r:id="rId166" display="&quot;Poor Marketing Execution - 14% of startups fail because of poor marketing efforts; founders focus all energy on product development and neglect critical marketing activities&quot;" xr:uid="{00000000-0004-0000-0500-0000AD000000}"/>
-    <hyperlink ref="T36" r:id="rId167" xr:uid="{00000000-0004-0000-0500-0000AE000000}"/>
-    <hyperlink ref="P37" r:id="rId168" xr:uid="{00000000-0004-0000-0500-0000AF000000}"/>
-    <hyperlink ref="R37" r:id="rId169" xr:uid="{00000000-0004-0000-0500-0000B0000000}"/>
-    <hyperlink ref="S37" r:id="rId170" xr:uid="{00000000-0004-0000-0500-0000B1000000}"/>
-    <hyperlink ref="T37" r:id="rId171" xr:uid="{00000000-0004-0000-0500-0000B2000000}"/>
-    <hyperlink ref="P38" r:id="rId172" xr:uid="{00000000-0004-0000-0500-0000B3000000}"/>
-    <hyperlink ref="R38" r:id="rId173" xr:uid="{00000000-0004-0000-0500-0000B4000000}"/>
-    <hyperlink ref="S38" r:id="rId174" xr:uid="{00000000-0004-0000-0500-0000B5000000}"/>
-    <hyperlink ref="T38" r:id="rId175" xr:uid="{00000000-0004-0000-0500-0000B6000000}"/>
-    <hyperlink ref="P39" r:id="rId176" xr:uid="{00000000-0004-0000-0500-0000B7000000}"/>
-    <hyperlink ref="R39" r:id="rId177" xr:uid="{00000000-0004-0000-0500-0000B8000000}"/>
-    <hyperlink ref="P40" r:id="rId178" xr:uid="{00000000-0004-0000-0500-0000B9000000}"/>
-    <hyperlink ref="R40" r:id="rId179" xr:uid="{00000000-0004-0000-0500-0000BA000000}"/>
-    <hyperlink ref="T40" r:id="rId180" xr:uid="{00000000-0004-0000-0500-0000BB000000}"/>
-    <hyperlink ref="P41" r:id="rId181" xr:uid="{00000000-0004-0000-0500-0000BC000000}"/>
-    <hyperlink ref="R41" r:id="rId182" xr:uid="{00000000-0004-0000-0500-0000BD000000}"/>
-    <hyperlink ref="S41" r:id="rId183" xr:uid="{00000000-0004-0000-0500-0000BE000000}"/>
-    <hyperlink ref="T41" r:id="rId184" xr:uid="{00000000-0004-0000-0500-0000BF000000}"/>
-    <hyperlink ref="P42" r:id="rId185" xr:uid="{00000000-0004-0000-0500-0000C0000000}"/>
-    <hyperlink ref="R42" r:id="rId186" xr:uid="{00000000-0004-0000-0500-0000C1000000}"/>
-    <hyperlink ref="T42" r:id="rId187" xr:uid="{00000000-0004-0000-0500-0000C2000000}"/>
-    <hyperlink ref="U42" r:id="rId188" xr:uid="{00000000-0004-0000-0500-0000C3000000}"/>
-    <hyperlink ref="G43" r:id="rId189" xr:uid="{00000000-0004-0000-0500-0000C4000000}"/>
-    <hyperlink ref="H43" r:id="rId190" xr:uid="{00000000-0004-0000-0500-0000C5000000}"/>
-    <hyperlink ref="I43" r:id="rId191" xr:uid="{00000000-0004-0000-0500-0000C6000000}"/>
-    <hyperlink ref="P43" r:id="rId192" xr:uid="{00000000-0004-0000-0500-0000C7000000}"/>
-    <hyperlink ref="R43" r:id="rId193" xr:uid="{00000000-0004-0000-0500-0000C8000000}"/>
-    <hyperlink ref="T43" r:id="rId194" xr:uid="{00000000-0004-0000-0500-0000C9000000}"/>
-    <hyperlink ref="U43" r:id="rId195" xr:uid="{00000000-0004-0000-0500-0000CA000000}"/>
-    <hyperlink ref="P44" r:id="rId196" xr:uid="{00000000-0004-0000-0500-0000CB000000}"/>
-    <hyperlink ref="R44" r:id="rId197" xr:uid="{00000000-0004-0000-0500-0000CC000000}"/>
-    <hyperlink ref="S44" r:id="rId198" xr:uid="{00000000-0004-0000-0500-0000CD000000}"/>
-    <hyperlink ref="T44" r:id="rId199" xr:uid="{00000000-0004-0000-0500-0000CE000000}"/>
-    <hyperlink ref="U44" r:id="rId200" xr:uid="{00000000-0004-0000-0500-0000CF000000}"/>
-    <hyperlink ref="P45" r:id="rId201" xr:uid="{00000000-0004-0000-0500-0000D0000000}"/>
-    <hyperlink ref="R45" r:id="rId202" xr:uid="{00000000-0004-0000-0500-0000D1000000}"/>
-    <hyperlink ref="S45" r:id="rId203" xr:uid="{00000000-0004-0000-0500-0000D2000000}"/>
-    <hyperlink ref="T45" r:id="rId204" xr:uid="{00000000-0004-0000-0500-0000D3000000}"/>
-    <hyperlink ref="P46" r:id="rId205" xr:uid="{00000000-0004-0000-0500-0000D4000000}"/>
-    <hyperlink ref="R46" r:id="rId206" xr:uid="{00000000-0004-0000-0500-0000D5000000}"/>
-    <hyperlink ref="S46" r:id="rId207" xr:uid="{00000000-0004-0000-0500-0000D6000000}"/>
-    <hyperlink ref="P47" r:id="rId208" xr:uid="{00000000-0004-0000-0500-0000D7000000}"/>
-    <hyperlink ref="P48" r:id="rId209" xr:uid="{00000000-0004-0000-0500-0000D8000000}"/>
-    <hyperlink ref="P49" r:id="rId210" xr:uid="{00000000-0004-0000-0500-0000D9000000}"/>
-    <hyperlink ref="P50" r:id="rId211" xr:uid="{00000000-0004-0000-0500-0000DA000000}"/>
-    <hyperlink ref="T50" r:id="rId212" xr:uid="{00000000-0004-0000-0500-0000DB000000}"/>
-    <hyperlink ref="P51" r:id="rId213" xr:uid="{00000000-0004-0000-0500-0000DC000000}"/>
-    <hyperlink ref="R51" r:id="rId214" xr:uid="{00000000-0004-0000-0500-0000DD000000}"/>
-    <hyperlink ref="T51" r:id="rId215" xr:uid="{00000000-0004-0000-0500-0000DE000000}"/>
-    <hyperlink ref="P52" r:id="rId216" xr:uid="{00000000-0004-0000-0500-0000DF000000}"/>
-    <hyperlink ref="R52" r:id="rId217" xr:uid="{00000000-0004-0000-0500-0000E0000000}"/>
-    <hyperlink ref="T52" r:id="rId218" xr:uid="{00000000-0004-0000-0500-0000E1000000}"/>
-    <hyperlink ref="G53" r:id="rId219" xr:uid="{00000000-0004-0000-0500-0000E2000000}"/>
-    <hyperlink ref="H53" r:id="rId220" xr:uid="{00000000-0004-0000-0500-0000E3000000}"/>
-    <hyperlink ref="P53" r:id="rId221" xr:uid="{00000000-0004-0000-0500-0000E4000000}"/>
-    <hyperlink ref="R53" r:id="rId222" display="&quot;Founder Quality - VCs look for founders with resilience, passion, and experience leading start-up teams — the right stuff matters more than the idea&quot;" xr:uid="{00000000-0004-0000-0500-0000E5000000}"/>
-    <hyperlink ref="S53" r:id="rId223" xr:uid="{00000000-0004-0000-0500-0000E6000000}"/>
-    <hyperlink ref="T53" r:id="rId224" xr:uid="{00000000-0004-0000-0500-0000E7000000}"/>
-    <hyperlink ref="U53" r:id="rId225" xr:uid="{00000000-0004-0000-0500-0000E8000000}"/>
-    <hyperlink ref="F54" r:id="rId226" xr:uid="{00000000-0004-0000-0500-0000E9000000}"/>
-    <hyperlink ref="G54" r:id="rId227" xr:uid="{00000000-0004-0000-0500-0000EA000000}"/>
-    <hyperlink ref="H54" r:id="rId228" xr:uid="{00000000-0004-0000-0500-0000EB000000}"/>
-    <hyperlink ref="I54" r:id="rId229" xr:uid="{00000000-0004-0000-0500-0000EC000000}"/>
-    <hyperlink ref="P54" r:id="rId230" xr:uid="{00000000-0004-0000-0500-0000ED000000}"/>
-    <hyperlink ref="R54" r:id="rId231" display="&quot;Governance Problems - Lack of foundational legal structure, compliance oversight, and board governance creates operational vulnerability and limits investment readiness&quot;" xr:uid="{00000000-0004-0000-0500-0000EE000000}"/>
-    <hyperlink ref="G55" r:id="rId232" xr:uid="{00000000-0004-0000-0500-0000EF000000}"/>
-    <hyperlink ref="P55" r:id="rId233" xr:uid="{00000000-0004-0000-0500-0000F0000000}"/>
-    <hyperlink ref="R55" r:id="rId234" display="&quot;Founder Quality - VCs look for founders with resilience, passion, and experience leading start-up teams   —   the right stuff matters more than the idea&quot;" xr:uid="{00000000-0004-0000-0500-0000F1000000}"/>
-    <hyperlink ref="G56" r:id="rId235" xr:uid="{00000000-0004-0000-0500-0000F2000000}"/>
-    <hyperlink ref="H56" r:id="rId236" xr:uid="{00000000-0004-0000-0500-0000F3000000}"/>
-    <hyperlink ref="P56" r:id="rId237" xr:uid="{00000000-0004-0000-0500-0000F4000000}"/>
-    <hyperlink ref="R56" r:id="rId238" xr:uid="{00000000-0004-0000-0500-0000F5000000}"/>
-    <hyperlink ref="S56" r:id="rId239" display="To expect communication naturally evolves with growth, for instance, is a false assumption many startup founders make. It’s obviously a lot easier to communicate changes and progress to a few other people, versus 10, 50 or even 1000 other people." xr:uid="{00000000-0004-0000-0500-0000F6000000}"/>
-    <hyperlink ref="T56" r:id="rId240" display="try to keep up with trends in your industry and be open to feedback that can help you improve the overall quality of your service or product." xr:uid="{00000000-0004-0000-0500-0000F7000000}"/>
-    <hyperlink ref="U56" r:id="rId241" xr:uid="{00000000-0004-0000-0500-0000F8000000}"/>
-    <hyperlink ref="G57" r:id="rId242" xr:uid="{00000000-0004-0000-0500-0000F9000000}"/>
-    <hyperlink ref="P57" r:id="rId243" xr:uid="{00000000-0004-0000-0500-0000FA000000}"/>
-    <hyperlink ref="R57" r:id="rId244" display="&quot;Market Adaptation Failure - Whether it's consumer preference shifts or black swan events like coronavirus, startups must adapt quickly to survive&quot;" xr:uid="{00000000-0004-0000-0500-0000FB000000}"/>
-    <hyperlink ref="T57" r:id="rId245" xr:uid="{00000000-0004-0000-0500-0000FC000000}"/>
-    <hyperlink ref="G58" r:id="rId246" xr:uid="{00000000-0004-0000-0500-0000FD000000}"/>
-    <hyperlink ref="H58" r:id="rId247" xr:uid="{00000000-0004-0000-0500-0000FE000000}"/>
-    <hyperlink ref="P58" r:id="rId248" xr:uid="{00000000-0004-0000-0500-0000FF000000}"/>
-    <hyperlink ref="R58" r:id="rId249" display="&quot;Pivot Necessity - 75% of startups change their initial ideas as the market landscape shifts; rigidly clinging to original plans guarantees failure&quot;" xr:uid="{00000000-0004-0000-0500-000000010000}"/>
-    <hyperlink ref="S58" r:id="rId250" xr:uid="{00000000-0004-0000-0500-000001010000}"/>
-    <hyperlink ref="T58" r:id="rId251" xr:uid="{00000000-0004-0000-0500-000002010000}"/>
-    <hyperlink ref="G59" r:id="rId252" xr:uid="{00000000-0004-0000-0500-000003010000}"/>
-    <hyperlink ref="H59" r:id="rId253" xr:uid="{00000000-0004-0000-0500-000004010000}"/>
-    <hyperlink ref="P59" r:id="rId254" xr:uid="{00000000-0004-0000-0500-000005010000}"/>
-    <hyperlink ref="R59" r:id="rId255" display="&quot;Customer-Led Development - We let the thousands decide what the millions will do — early customer feedback guides mass market decisions&quot;" xr:uid="{00000000-0004-0000-0500-000006010000}"/>
-    <hyperlink ref="T59" r:id="rId256" xr:uid="{00000000-0004-0000-0500-000007010000}"/>
-    <hyperlink ref="G60" r:id="rId257" xr:uid="{00000000-0004-0000-0500-000008010000}"/>
-    <hyperlink ref="H60" r:id="rId258" xr:uid="{00000000-0004-0000-0500-000009010000}"/>
-    <hyperlink ref="P60" r:id="rId259" xr:uid="{00000000-0004-0000-0500-00000A010000}"/>
-    <hyperlink ref="R60" r:id="rId260" display="&quot;Customer-Led Development - We let the thousands decide what the millions will do   —   early customer feedback guides mass market decisions&quot;" xr:uid="{00000000-0004-0000-0500-00000B010000}"/>
-    <hyperlink ref="T60" r:id="rId261" xr:uid="{00000000-0004-0000-0500-00000C010000}"/>
-    <hyperlink ref="J61" r:id="rId262" xr:uid="{00000000-0004-0000-0500-00000D010000}"/>
-    <hyperlink ref="K61" r:id="rId263" xr:uid="{00000000-0004-0000-0500-00000E010000}"/>
-    <hyperlink ref="L61" r:id="rId264" xr:uid="{00000000-0004-0000-0500-00000F010000}"/>
-    <hyperlink ref="G62" r:id="rId265" xr:uid="{00000000-0004-0000-0500-000013010000}"/>
-    <hyperlink ref="H62" r:id="rId266" xr:uid="{00000000-0004-0000-0500-000014010000}"/>
-    <hyperlink ref="P62" r:id="rId267" xr:uid="{00000000-0004-0000-0500-000015010000}"/>
-    <hyperlink ref="R62" r:id="rId268" xr:uid="{00000000-0004-0000-0500-000016010000}"/>
-    <hyperlink ref="S62" r:id="rId269" xr:uid="{00000000-0004-0000-0500-000017010000}"/>
-    <hyperlink ref="T62" r:id="rId270" xr:uid="{00000000-0004-0000-0500-000018010000}"/>
-    <hyperlink ref="U62" r:id="rId271" xr:uid="{00000000-0004-0000-0500-000019010000}"/>
-    <hyperlink ref="G61" r:id="rId272" xr:uid="{00000000-0004-0000-0500-00001A010000}"/>
-    <hyperlink ref="H61" r:id="rId273" xr:uid="{00000000-0004-0000-0500-00001B010000}"/>
-    <hyperlink ref="I61" r:id="rId274" xr:uid="{00000000-0004-0000-0500-00001C010000}"/>
-    <hyperlink ref="P61" r:id="rId275" xr:uid="{00000000-0004-0000-0500-00001D010000}"/>
-    <hyperlink ref="S61" r:id="rId276" display="&quot;Innovation Failure - MySpace failed to innovate, didn't track young users' rapidly changing habits, and quickly fell behind Facebook&quot;" xr:uid="{00000000-0004-0000-0500-00001E010000}"/>
-    <hyperlink ref="T61" r:id="rId277" xr:uid="{00000000-0004-0000-0500-00001F010000}"/>
-    <hyperlink ref="P63" r:id="rId278" xr:uid="{00000000-0004-0000-0500-000020010000}"/>
-    <hyperlink ref="R63" r:id="rId279" display="&quot;Insufficient Network/Allies - Lack of referral sources and industry connections limits growth acceleration and credibility&quot;" xr:uid="{00000000-0004-0000-0500-000021010000}"/>
-    <hyperlink ref="T64" r:id="rId280" display="Ensure you have a strong presence on the right social media channels and utilize them to their fullest potential." xr:uid="{00000000-0004-0000-0500-000022010000}"/>
-    <hyperlink ref="G64" r:id="rId281" xr:uid="{00000000-0004-0000-0500-000023010000}"/>
-    <hyperlink ref="H64" r:id="rId282" xr:uid="{00000000-0004-0000-0500-000024010000}"/>
-    <hyperlink ref="P64" r:id="rId283" xr:uid="{00000000-0004-0000-0500-000025010000}"/>
-    <hyperlink ref="R64" r:id="rId284" display="&quot;Customer Service Orientation (66% of sample) - Prioritized new customer acquisition over retention; focused on technological solutions rather than customer needs&quot;" xr:uid="{00000000-0004-0000-0500-000026010000}"/>
-    <hyperlink ref="G65" r:id="rId285" xr:uid="{00000000-0004-0000-0500-000027010000}"/>
-    <hyperlink ref="H65" r:id="rId286" xr:uid="{00000000-0004-0000-0500-000028010000}"/>
-    <hyperlink ref="I65" r:id="rId287" xr:uid="{00000000-0004-0000-0500-000029010000}"/>
-    <hyperlink ref="P65" r:id="rId288" xr:uid="{00000000-0004-0000-0500-00002A010000}"/>
-    <hyperlink ref="R65" r:id="rId289" display="&quot;Customer Service Orientation (66% of sample) - Prioritised new customer acquisition over retention; focused on technological solutions rather than customer needs&quot;" xr:uid="{00000000-0004-0000-0500-00002B010000}"/>
-    <hyperlink ref="P66" r:id="rId290" xr:uid="{00000000-0004-0000-0500-00002C010000}"/>
-    <hyperlink ref="R66" r:id="rId291" xr:uid="{00000000-0004-0000-0500-00002D010000}"/>
-    <hyperlink ref="S66" r:id="rId292" xr:uid="{00000000-0004-0000-0500-00002E010000}"/>
-    <hyperlink ref="T66" r:id="rId293" display="seek advice from experienced entrepreneurs who have gone through the process before, as they can provide valuable insight and feedback." xr:uid="{00000000-0004-0000-0500-00002F010000}"/>
-    <hyperlink ref="P67" r:id="rId294" xr:uid="{00000000-0004-0000-0500-000030010000}"/>
-    <hyperlink ref="R67" r:id="rId295" xr:uid="{00000000-0004-0000-0500-000031010000}"/>
-    <hyperlink ref="S67" r:id="rId296" xr:uid="{00000000-0004-0000-0500-000032010000}"/>
-    <hyperlink ref="T67" r:id="rId297" display="Analyzing your overall business performance is also important. If your business goals, product development goals, marketing iniatives, and team communications are becoming confusing or uncertain, this won’t go over well in your next pitch meeting. Investors want to see a clear vision, a clear pathway to success, and evidence that you can follow through." xr:uid="{00000000-0004-0000-0500-000033010000}"/>
-    <hyperlink ref="P68" r:id="rId298" xr:uid="{00000000-0004-0000-0500-000034010000}"/>
-    <hyperlink ref="R68" r:id="rId299" xr:uid="{00000000-0004-0000-0500-000035010000}"/>
-    <hyperlink ref="S68" r:id="rId300" xr:uid="{00000000-0004-0000-0500-000036010000}"/>
-    <hyperlink ref="P69" r:id="rId301" xr:uid="{00000000-0004-0000-0500-000037010000}"/>
-    <hyperlink ref="R69" r:id="rId302" xr:uid="{00000000-0004-0000-0500-000038010000}"/>
-    <hyperlink ref="S69" r:id="rId303" xr:uid="{00000000-0004-0000-0500-000039010000}"/>
-    <hyperlink ref="P70" r:id="rId304" xr:uid="{00000000-0004-0000-0500-00003A010000}"/>
-    <hyperlink ref="R70" r:id="rId305" xr:uid="{00000000-0004-0000-0500-00003B010000}"/>
-    <hyperlink ref="S70" r:id="rId306" xr:uid="{00000000-0004-0000-0500-00003C010000}"/>
-    <hyperlink ref="P71" r:id="rId307" xr:uid="{00000000-0004-0000-0500-00003D010000}"/>
-    <hyperlink ref="T71" r:id="rId308" xr:uid="{00000000-0004-0000-0500-00003E010000}"/>
-    <hyperlink ref="P72" r:id="rId309" xr:uid="{00000000-0004-0000-0500-00003F010000}"/>
-    <hyperlink ref="R72" r:id="rId310" xr:uid="{00000000-0004-0000-0500-000040010000}"/>
-    <hyperlink ref="T72" r:id="rId311" xr:uid="{00000000-0004-0000-0500-000041010000}"/>
-    <hyperlink ref="P73" r:id="rId312" xr:uid="{00000000-0004-0000-0500-000042010000}"/>
-    <hyperlink ref="R73" r:id="rId313" xr:uid="{00000000-0004-0000-0500-000043010000}"/>
-    <hyperlink ref="T73" r:id="rId314" display="Startups should concentrate on one core offering, perfect it, and then consider expanding. Maintaining focus and prioritizing resources on a single product or service can help startups avoid spreading themselves too thin and ensure they deliver exceptional value to their customers." xr:uid="{00000000-0004-0000-0500-000044010000}"/>
-    <hyperlink ref="P74" r:id="rId315" xr:uid="{00000000-0004-0000-0500-000045010000}"/>
-    <hyperlink ref="R74" r:id="rId316" xr:uid="{00000000-0004-0000-0500-000046010000}"/>
-    <hyperlink ref="T74" r:id="rId317" xr:uid="{00000000-0004-0000-0500-000047010000}"/>
-    <hyperlink ref="U74" r:id="rId318" xr:uid="{00000000-0004-0000-0500-000048010000}"/>
-    <hyperlink ref="P75" r:id="rId319" xr:uid="{00000000-0004-0000-0500-000049010000}"/>
-    <hyperlink ref="R75" r:id="rId320" xr:uid="{00000000-0004-0000-0500-00004A010000}"/>
-    <hyperlink ref="U75" r:id="rId321" xr:uid="{00000000-0004-0000-0500-00004B010000}"/>
-    <hyperlink ref="P76" r:id="rId322" xr:uid="{00000000-0004-0000-0500-00004C010000}"/>
-    <hyperlink ref="U76" r:id="rId323" xr:uid="{00000000-0004-0000-0500-00004D010000}"/>
-    <hyperlink ref="P77" r:id="rId324" xr:uid="{00000000-0004-0000-0500-00004E010000}"/>
-    <hyperlink ref="P78" r:id="rId325" xr:uid="{00000000-0004-0000-0500-00004F010000}"/>
-    <hyperlink ref="T78" r:id="rId326" xr:uid="{00000000-0004-0000-0500-000050010000}"/>
-    <hyperlink ref="P79" r:id="rId327" xr:uid="{00000000-0004-0000-0500-000051010000}"/>
-    <hyperlink ref="P80" r:id="rId328" xr:uid="{00000000-0004-0000-0500-000052010000}"/>
-    <hyperlink ref="P81" r:id="rId329" xr:uid="{00000000-0004-0000-0500-000053010000}"/>
-    <hyperlink ref="R81" r:id="rId330" xr:uid="{00000000-0004-0000-0500-000054010000}"/>
-    <hyperlink ref="T81" r:id="rId331" xr:uid="{00000000-0004-0000-0500-000055010000}"/>
-    <hyperlink ref="G82" r:id="rId332" xr:uid="{00000000-0004-0000-0500-000056010000}"/>
-    <hyperlink ref="H82" r:id="rId333" xr:uid="{00000000-0004-0000-0500-000057010000}"/>
-    <hyperlink ref="P82" r:id="rId334" xr:uid="{00000000-0004-0000-0500-000058010000}"/>
-    <hyperlink ref="R82" r:id="rId335" xr:uid="{00000000-0004-0000-0500-000059010000}"/>
-    <hyperlink ref="S82" r:id="rId336" xr:uid="{00000000-0004-0000-0500-00005A010000}"/>
-    <hyperlink ref="T82" r:id="rId337" xr:uid="{00000000-0004-0000-0500-00005B010000}"/>
-    <hyperlink ref="U82" r:id="rId338" xr:uid="{00000000-0004-0000-0500-00005C010000}"/>
-    <hyperlink ref="G83" r:id="rId339" xr:uid="{00000000-0004-0000-0500-00005D010000}"/>
-    <hyperlink ref="H83" r:id="rId340" xr:uid="{00000000-0004-0000-0500-00005E010000}"/>
-    <hyperlink ref="P83" r:id="rId341" xr:uid="{00000000-0004-0000-0500-00005F010000}"/>
-    <hyperlink ref="R83" r:id="rId342" display="&quot;Founder Over-Extension - I quickly became stretched too thin and lost connection with staff; the entire enterprise began to lose focus and flounder&quot;" xr:uid="{00000000-0004-0000-0500-000060010000}"/>
-    <hyperlink ref="T83" r:id="rId343" xr:uid="{00000000-0004-0000-0500-000061010000}"/>
-    <hyperlink ref="H84" r:id="rId344" xr:uid="{00000000-0004-0000-0500-000062010000}"/>
-    <hyperlink ref="I84" r:id="rId345" xr:uid="{00000000-0004-0000-0500-000063010000}"/>
-    <hyperlink ref="J84" r:id="rId346" xr:uid="{00000000-0004-0000-0500-000064010000}"/>
-    <hyperlink ref="P84" r:id="rId347" xr:uid="{00000000-0004-0000-0500-000065010000}"/>
-    <hyperlink ref="R84" r:id="rId348" display="&quot;Team Problems - 23% of startups fail from missing expertise and weak leadership. Early-stage teams lack experienced leaders who can scale operations, resulting in founder burnout and operational chaos as complexity increases.&quot;" xr:uid="{00000000-0004-0000-0500-000066010000}"/>
-    <hyperlink ref="S84" r:id="rId349" display="&quot;Insufficient Network/Allies - Lack of referral sources and industry connections limits growth acceleration and credibility&quot;" xr:uid="{00000000-0004-0000-0500-000067010000}"/>
-    <hyperlink ref="T84" r:id="rId350" display="seek advice from experienced entrepreneurs who have gone through the process before, as they can provide valuable insight and feedback." xr:uid="{00000000-0004-0000-0500-000068010000}"/>
-    <hyperlink ref="U84" r:id="rId351" xr:uid="{00000000-0004-0000-0500-000069010000}"/>
-    <hyperlink ref="G85" r:id="rId352" xr:uid="{00000000-0004-0000-0500-00006A010000}"/>
-    <hyperlink ref="H85" r:id="rId353" xr:uid="{00000000-0004-0000-0500-00006B010000}"/>
-    <hyperlink ref="P85" r:id="rId354" xr:uid="{00000000-0004-0000-0500-00006C010000}"/>
-    <hyperlink ref="R85" r:id="rId355" xr:uid="{00000000-0004-0000-0500-00006D010000}"/>
-    <hyperlink ref="S85" r:id="rId356" display="&quot;Communication Doesn't Scale Naturally - False assumption that communication evolves automatically; communicating changes to 1000 people differs fundamentally from 10&quot;" xr:uid="{00000000-0004-0000-0500-00006E010000}"/>
-    <hyperlink ref="T85" r:id="rId357" display="Analyzing your overall business performance is also important. If your business goals, product development goals, marketing iniatives, and team communications are becoming confusing or uncertain, this won’t go over well in your next pitch meeting. Investors want to see a clear vision, a clear pathway to success, and evidence that you can follow through." xr:uid="{00000000-0004-0000-0500-00006F010000}"/>
-    <hyperlink ref="U85" r:id="rId358" xr:uid="{00000000-0004-0000-0500-000070010000}"/>
-    <hyperlink ref="G86" r:id="rId359" xr:uid="{00000000-0004-0000-0500-000071010000}"/>
-    <hyperlink ref="H86" r:id="rId360" xr:uid="{00000000-0004-0000-0500-000072010000}"/>
-    <hyperlink ref="P86" r:id="rId361" xr:uid="{00000000-0004-0000-0500-000073010000}"/>
-    <hyperlink ref="R86" r:id="rId362" display="&quot;Lacking Scalable Infrastructure - Failing to systematically establish communication systems, IT redundancy, and operational procedures for growing team sise. You need to invest in your company's communication infrastructure.&quot;" xr:uid="{00000000-0004-0000-0500-000074010000}"/>
-    <hyperlink ref="G87" r:id="rId363" xr:uid="{00000000-0004-0000-0500-000075010000}"/>
-    <hyperlink ref="P87" r:id="rId364" xr:uid="{00000000-0004-0000-0500-000076010000}"/>
-    <hyperlink ref="R87" r:id="rId365" display="&quot;Over-Customising for Customers - Saying yes to every customer feature request during scale-up creates over-promising, under-delivering, and unsustainable complexity&quot;" xr:uid="{00000000-0004-0000-0500-000077010000}"/>
-    <hyperlink ref="S87" r:id="rId366" xr:uid="{00000000-0004-0000-0500-000078010000}"/>
-    <hyperlink ref="G88" r:id="rId367" xr:uid="{00000000-0004-0000-0500-000079010000}"/>
-    <hyperlink ref="H88" r:id="rId368" xr:uid="{00000000-0004-0000-0500-00007A010000}"/>
-    <hyperlink ref="P88" r:id="rId369" xr:uid="{00000000-0004-0000-0500-00007B010000}"/>
-    <hyperlink ref="R88" r:id="rId370" display="&quot;Pivot Failure - Textbook example: Blockbuster had 9,000+ stores and owned movie-rental market but failed to pivot when market shifted&quot;" xr:uid="{00000000-0004-0000-0500-00007C010000}"/>
-    <hyperlink ref="G89" r:id="rId371" xr:uid="{00000000-0004-0000-0500-00007D010000}"/>
-    <hyperlink ref="H89" r:id="rId372" xr:uid="{00000000-0004-0000-0500-00007E010000}"/>
-    <hyperlink ref="P89" r:id="rId373" xr:uid="{00000000-0004-0000-0500-00007F010000}"/>
-    <hyperlink ref="R89" r:id="rId374" display="&quot;Leadership Dysfunction - Dysfunction at the top quickly infects the entire organisation, draining morale and destroying culture&quot;" xr:uid="{00000000-0004-0000-0500-000080010000}"/>
-    <hyperlink ref="T89" r:id="rId375" xr:uid="{00000000-0004-0000-0500-000081010000}"/>
-    <hyperlink ref="U89" r:id="rId376" xr:uid="{00000000-0004-0000-0500-000082010000}"/>
-    <hyperlink ref="G90" r:id="rId377" xr:uid="{00000000-0004-0000-0500-000083010000}"/>
-    <hyperlink ref="P90" r:id="rId378" xr:uid="{00000000-0004-0000-0500-000084010000}"/>
-    <hyperlink ref="R90" r:id="rId379" xr:uid="{00000000-0004-0000-0500-000085010000}"/>
-    <hyperlink ref="S90" r:id="rId380" xr:uid="{00000000-0004-0000-0500-000086010000}"/>
-    <hyperlink ref="T90" r:id="rId381" xr:uid="{00000000-0004-0000-0500-000087010000}"/>
-    <hyperlink ref="G91" r:id="rId382" xr:uid="{00000000-0004-0000-0500-000088010000}"/>
-    <hyperlink ref="H91" r:id="rId383" xr:uid="{00000000-0004-0000-0500-000089010000}"/>
-    <hyperlink ref="P91" r:id="rId384" xr:uid="{00000000-0004-0000-0500-00008A010000}"/>
-    <hyperlink ref="R91" r:id="rId385" display="Startups fail by spreading too thin across multiple markets/channels simultaneously. Dominate one market before expanding to next. - CB Insights" xr:uid="{00000000-0004-0000-0500-00008B010000}"/>
-    <hyperlink ref="S91" r:id="rId386" display="&quot;Offering Too Many Services - Trying to serve all markets increases operational complexity and diverts from core purpose&quot;" xr:uid="{00000000-0004-0000-0500-00008C010000}"/>
-    <hyperlink ref="T91" r:id="rId387" display="Startups should concentrate on one core offering, perfect it, and then consider expanding. Maintaining focus and prioritizing resources on a single product or service can help startups avoid spreading themselves too thin and ensure they deliver exceptional value to their customers." xr:uid="{00000000-0004-0000-0500-00008D010000}"/>
-    <hyperlink ref="G92" r:id="rId388" xr:uid="{00000000-0004-0000-0500-00008E010000}"/>
-    <hyperlink ref="H92" r:id="rId389" xr:uid="{00000000-0004-0000-0500-00008F010000}"/>
-    <hyperlink ref="I92" r:id="rId390" xr:uid="{00000000-0004-0000-0500-000090010000}"/>
-    <hyperlink ref="P92" r:id="rId391" xr:uid="{00000000-0004-0000-0500-000091010000}"/>
-    <hyperlink ref="R92" r:id="rId392" display="Referrals are an especially powerful tool for growing a startup. Unlike traditional forms of marketing, referrals are backed by trust and personal endorsements. This type of marketing not only spreads awareness of your business but also enhances its credibility." xr:uid="{00000000-0004-0000-0500-000092010000}"/>
-    <hyperlink ref="T92" r:id="rId393" xr:uid="{00000000-0004-0000-0500-000093010000}"/>
-    <hyperlink ref="U92" r:id="rId394" xr:uid="{00000000-0004-0000-0500-000094010000}"/>
-    <hyperlink ref="G93" r:id="rId395" xr:uid="{00000000-0004-0000-0500-000095010000}"/>
-    <hyperlink ref="H93" r:id="rId396" xr:uid="{00000000-0004-0000-0500-000096010000}"/>
-    <hyperlink ref="I93" r:id="rId397" xr:uid="{00000000-0004-0000-0500-000097010000}"/>
-    <hyperlink ref="P93" r:id="rId398" xr:uid="{00000000-0004-0000-0500-000098010000}"/>
-    <hyperlink ref="R93" r:id="rId399" display="&quot;Referral Power - Referrals backed by trust and personal endorsements spread awareness while enhancing credibility, unlike traditional marketing&quot;" xr:uid="{00000000-0004-0000-0500-000099010000}"/>
-    <hyperlink ref="G94" r:id="rId400" xr:uid="{00000000-0004-0000-0500-00009A010000}"/>
-    <hyperlink ref="H94" r:id="rId401" xr:uid="{00000000-0004-0000-0500-00009B010000}"/>
-    <hyperlink ref="I94" r:id="rId402" xr:uid="{00000000-0004-0000-0500-00009C010000}"/>
-    <hyperlink ref="P94" r:id="rId403" xr:uid="{00000000-0004-0000-0500-00009D010000}"/>
-    <hyperlink ref="R94" r:id="rId404" display="&quot;Competitive Reality - Assume competitors already exist; your product may not be as unique as you think. Differentiation requires deliberate strategy&quot;" xr:uid="{00000000-0004-0000-0500-00009E010000}"/>
-    <hyperlink ref="G95" r:id="rId405" xr:uid="{00000000-0004-0000-0500-00009F010000}"/>
-    <hyperlink ref="H95" r:id="rId406" location="the-best-marketing-frameworks" xr:uid="{00000000-0004-0000-0500-0000A0010000}"/>
-    <hyperlink ref="I95" r:id="rId407" xr:uid="{00000000-0004-0000-0500-0000A1010000}"/>
-    <hyperlink ref="P95" r:id="rId408" xr:uid="{00000000-0004-0000-0500-0000A2010000}"/>
-    <hyperlink ref="R95" r:id="rId409" display="&quot;Single-Channel Risk - Putting all growth efforts in one channel basket creates vulnerability; channel diversification is essential for scaling&quot;" xr:uid="{00000000-0004-0000-0500-0000A3010000}"/>
-    <hyperlink ref="P96" r:id="rId410" xr:uid="{00000000-0004-0000-0500-0000A4010000}"/>
-    <hyperlink ref="R96" r:id="rId411" xr:uid="{00000000-0004-0000-0500-0000A5010000}"/>
-    <hyperlink ref="T96" r:id="rId412" xr:uid="{00000000-0004-0000-0500-0000A6010000}"/>
-    <hyperlink ref="P97" r:id="rId413" xr:uid="{00000000-0004-0000-0500-0000A7010000}"/>
-    <hyperlink ref="R97" r:id="rId414" xr:uid="{00000000-0004-0000-0500-0000A8010000}"/>
-    <hyperlink ref="T97" r:id="rId415" xr:uid="{00000000-0004-0000-0500-0000A9010000}"/>
-    <hyperlink ref="P98" r:id="rId416" xr:uid="{00000000-0004-0000-0500-0000AA010000}"/>
-    <hyperlink ref="R98" r:id="rId417" xr:uid="{00000000-0004-0000-0500-0000AB010000}"/>
-    <hyperlink ref="P99" r:id="rId418" xr:uid="{00000000-0004-0000-0500-0000AC010000}"/>
-    <hyperlink ref="P100" r:id="rId419" xr:uid="{00000000-0004-0000-0500-0000AD010000}"/>
-    <hyperlink ref="R100" r:id="rId420" xr:uid="{00000000-0004-0000-0500-0000AE010000}"/>
-    <hyperlink ref="T100" r:id="rId421" xr:uid="{00000000-0004-0000-0500-0000AF010000}"/>
-    <hyperlink ref="P101" r:id="rId422" xr:uid="{00000000-0004-0000-0500-0000B0010000}"/>
-    <hyperlink ref="R101" r:id="rId423" xr:uid="{00000000-0004-0000-0500-0000B1010000}"/>
-    <hyperlink ref="T101" r:id="rId424" xr:uid="{00000000-0004-0000-0500-0000B2010000}"/>
-    <hyperlink ref="P102" r:id="rId425" xr:uid="{00000000-0004-0000-0500-0000B3010000}"/>
-    <hyperlink ref="R102" r:id="rId426" xr:uid="{00000000-0004-0000-0500-0000B4010000}"/>
-    <hyperlink ref="T102" r:id="rId427" xr:uid="{00000000-0004-0000-0500-0000B5010000}"/>
-    <hyperlink ref="U102" r:id="rId428" xr:uid="{00000000-0004-0000-0500-0000B6010000}"/>
-    <hyperlink ref="P103" r:id="rId429" xr:uid="{00000000-0004-0000-0500-0000B7010000}"/>
-    <hyperlink ref="R103" r:id="rId430" xr:uid="{00000000-0004-0000-0500-0000B8010000}"/>
-    <hyperlink ref="T103" r:id="rId431" xr:uid="{00000000-0004-0000-0500-0000B9010000}"/>
-    <hyperlink ref="U103" r:id="rId432" xr:uid="{00000000-0004-0000-0500-0000BA010000}"/>
-    <hyperlink ref="O104" r:id="rId433" xr:uid="{00000000-0004-0000-0500-0000BB010000}"/>
-    <hyperlink ref="P104" r:id="rId434" xr:uid="{00000000-0004-0000-0500-0000BC010000}"/>
-    <hyperlink ref="R104" r:id="rId435" display="Long-term goals are often overlooked in startups for reasons (or excuses) of agility but if you want to move fast, you need to know where you are going. You have to be able to make quick but smart decisions. And this requires a clear sense of direction." xr:uid="{00000000-0004-0000-0500-0000BD010000}"/>
-    <hyperlink ref="S104" r:id="rId436" xr:uid="{00000000-0004-0000-0500-0000BE010000}"/>
-    <hyperlink ref="T104" r:id="rId437" display="some startups rely too heavily on their original team members, who, despite being capable of managing early-stage growth, may lack the necessary skills and experience for later stages. That dependence can hold back a startup’s development and prevent it from achieving its full potential. Startups need to strike a balance between leveraging fresh perspectives with the insights of existing employees." xr:uid="{00000000-0004-0000-0500-0000BF010000}"/>
-    <hyperlink ref="U104" r:id="rId438" xr:uid="{00000000-0004-0000-0500-0000C0010000}"/>
-    <hyperlink ref="P105" r:id="rId439" xr:uid="{00000000-0004-0000-0500-0000C1010000}"/>
-    <hyperlink ref="R105" r:id="rId440" xr:uid="{00000000-0004-0000-0500-0000C2010000}"/>
-    <hyperlink ref="S105" r:id="rId441" xr:uid="{00000000-0004-0000-0500-0000C3010000}"/>
-    <hyperlink ref="T105" r:id="rId442" xr:uid="{00000000-0004-0000-0500-0000C4010000}"/>
-    <hyperlink ref="U105" r:id="rId443" xr:uid="{00000000-0004-0000-0500-0000C5010000}"/>
-    <hyperlink ref="P106" r:id="rId444" xr:uid="{00000000-0004-0000-0500-0000C6010000}"/>
-    <hyperlink ref="R106" r:id="rId445" xr:uid="{00000000-0004-0000-0500-0000C7010000}"/>
-    <hyperlink ref="T106" r:id="rId446" display="Encourage an environment of transparency, constructive feedback, and empathy among your team. Implementing feedback surveys (and listening to the feedback) or setting up times for team members to communicate and discuss their disagreements is essential for resolving conflicts. " xr:uid="{00000000-0004-0000-0500-0000C8010000}"/>
-    <hyperlink ref="U106" r:id="rId447" xr:uid="{00000000-0004-0000-0500-0000C9010000}"/>
-    <hyperlink ref="P107" r:id="rId448" xr:uid="{00000000-0004-0000-0500-0000CA010000}"/>
-    <hyperlink ref="R107" r:id="rId449" xr:uid="{00000000-0004-0000-0500-0000CB010000}"/>
-    <hyperlink ref="T107" r:id="rId450" xr:uid="{00000000-0004-0000-0500-0000CC010000}"/>
-    <hyperlink ref="U107" r:id="rId451" xr:uid="{00000000-0004-0000-0500-0000CD010000}"/>
-    <hyperlink ref="P108" r:id="rId452" xr:uid="{00000000-0004-0000-0500-0000CE010000}"/>
-    <hyperlink ref="R108" r:id="rId453" xr:uid="{00000000-0004-0000-0500-0000CF010000}"/>
-    <hyperlink ref="P109" r:id="rId454" xr:uid="{00000000-0004-0000-0500-0000D0010000}"/>
-    <hyperlink ref="R109" r:id="rId455" xr:uid="{00000000-0004-0000-0500-0000D1010000}"/>
-    <hyperlink ref="P110" r:id="rId456" xr:uid="{00000000-0004-0000-0500-0000D2010000}"/>
-    <hyperlink ref="R110" r:id="rId457" xr:uid="{00000000-0004-0000-0500-0000D3010000}"/>
-    <hyperlink ref="P111" r:id="rId458" xr:uid="{00000000-0004-0000-0500-0000D4010000}"/>
-    <hyperlink ref="R111" r:id="rId459" xr:uid="{00000000-0004-0000-0500-0000D5010000}"/>
-    <hyperlink ref="P112" r:id="rId460" xr:uid="{00000000-0004-0000-0500-0000D6010000}"/>
-    <hyperlink ref="R112" r:id="rId461" xr:uid="{00000000-0004-0000-0500-0000D7010000}"/>
-    <hyperlink ref="S112" r:id="rId462" xr:uid="{00000000-0004-0000-0500-0000D8010000}"/>
-    <hyperlink ref="P113" r:id="rId463" xr:uid="{00000000-0004-0000-0500-0000D9010000}"/>
-    <hyperlink ref="I10" r:id="rId464" xr:uid="{DC1CC40C-76BF-4151-B4AE-6B27A4A2CA83}"/>
-    <hyperlink ref="L17" r:id="rId465" xr:uid="{86177E8A-8D81-4E6A-9857-7126C272F5F9}"/>
-    <hyperlink ref="K18" r:id="rId466" xr:uid="{90524FBC-4648-460B-AF07-40CF07362549}"/>
-    <hyperlink ref="L18" r:id="rId467" xr:uid="{45C73B90-FD7A-47AC-8435-288C2341EA2C}"/>
-    <hyperlink ref="L24" r:id="rId468" xr:uid="{841EE744-F15D-4AD1-B723-3561AEDAD835}"/>
-    <hyperlink ref="L25" r:id="rId469" xr:uid="{06FA8D96-68AE-46E7-A79A-4A8DC12AD08C}"/>
-    <hyperlink ref="I28" r:id="rId470" display="PESTLE analysis" xr:uid="{0D490440-4354-4655-A3DD-EE81F7C6055A}"/>
-    <hyperlink ref="K39" r:id="rId471" xr:uid="{2ACB092F-8BB8-4B6E-9A08-8A35F74EE22A}"/>
-    <hyperlink ref="L39" r:id="rId472" xr:uid="{B625F6C3-BACC-46E9-88C0-E746813555A7}"/>
-    <hyperlink ref="K41" r:id="rId473" xr:uid="{3741B1DB-8273-4F29-B54C-88D8A0435455}"/>
-    <hyperlink ref="L41" r:id="rId474" xr:uid="{BA1B52BE-9404-49FC-A335-ED0787CA4FAA}"/>
-    <hyperlink ref="K43" r:id="rId475" location=":~:text=The%20Double%20Diamond%20is%20a,%E2%80%94%20solutions%20that%20work%20(converging)" xr:uid="{8B1BF22B-2F01-4A9F-8BAC-3F87FC74ACB7}"/>
-    <hyperlink ref="K44" r:id="rId476" location=":~:text=They%20focus%20on%20people%20and,Finally%2C%20they%20do%20small%20interventions." xr:uid="{F923DCE5-903C-4C42-B606-F89F10046C40}"/>
-    <hyperlink ref="H5" r:id="rId477" xr:uid="{BE6E9774-A880-45F8-8ED1-2C6482C46851}"/>
-    <hyperlink ref="G5" r:id="rId478" xr:uid="{2C4CBDFB-296B-4ADF-A1BE-EE19D2A7F865}"/>
-    <hyperlink ref="J7" r:id="rId479" xr:uid="{92D8F356-A1FF-4F87-B03D-C34C7A09C64E}"/>
-    <hyperlink ref="K7" r:id="rId480" xr:uid="{6825C89D-5444-4995-9806-D6E89DD5CBE7}"/>
-    <hyperlink ref="H9" r:id="rId481" xr:uid="{9A76F0FB-C178-46D3-A7D8-9024FAAF9D97}"/>
-    <hyperlink ref="G9" r:id="rId482" xr:uid="{630C9616-0E5C-4651-A337-654125678644}"/>
-    <hyperlink ref="J10" r:id="rId483" xr:uid="{3C841678-6F8C-4428-90E6-C893A557463E}"/>
-    <hyperlink ref="H10" r:id="rId484" xr:uid="{132EBC56-BDE1-4359-B18E-6DA3FD5113BF}"/>
-    <hyperlink ref="I31" r:id="rId485" xr:uid="{00000000-0004-0000-0500-000083000000}"/>
-    <hyperlink ref="T32" r:id="rId486" xr:uid="{CAD8C31C-98EF-4F8F-A865-FB61F17AA62A}"/>
-    <hyperlink ref="R32" r:id="rId487" xr:uid="{B6BA9457-7FC4-4838-B63A-C209AFC28F78}"/>
-    <hyperlink ref="H57" r:id="rId488" display="PESTLE analysis" xr:uid="{706B041A-8422-4768-8FF3-DB11748C24A7}"/>
-    <hyperlink ref="N61" r:id="rId489" xr:uid="{03235505-13B9-4900-8D97-98A45CC7E9CE}"/>
-    <hyperlink ref="R61" r:id="rId490" display="To expect communication naturally evolves with growth, for instance, is a false assumption many startup founders make. It’s obviously a lot easier to communicate changes and progress to a few other people, versus 10, 50 or even 1000 other people." xr:uid="{F719F4D6-E9DA-44FB-BA73-3F801A64E73B}"/>
-    <hyperlink ref="H90" r:id="rId491" xr:uid="{C8DC8E67-047A-42D9-99A3-7989946866BB}"/>
-    <hyperlink ref="G10" r:id="rId492" xr:uid="{6B4FE341-660E-4816-8C8E-F3E6F606E3AF}"/>
-    <hyperlink ref="G6" r:id="rId493" xr:uid="{9CFCAFB9-3246-4720-941D-AC16CBC47BC8}"/>
-    <hyperlink ref="K9" r:id="rId494" display="Jobs To Be Done Framework" xr:uid="{5D955235-3777-417A-83C7-9F8C7EE7F5B3}"/>
-    <hyperlink ref="J8" r:id="rId495" display="Pilot Program Framework" xr:uid="{49F44223-C389-4AC9-9EC1-20DEAF774550}"/>
-    <hyperlink ref="K10" r:id="rId496" xr:uid="{86063A33-ACBC-4811-B4E1-83A5DA720088}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="P2" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="R2" r:id="rId5" display="&quot;Governance Problems - Lack of foundational legal structure, compliance oversight, and board governance creates operational vulnerability and limits investment readiness&quot;" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="G3" r:id="rId6" display="Shareholders Agreement Template (if Team)" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="P3" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="R3" r:id="rId8" display="&quot;Shareholder Disagreement - Differences of opinion among founders create disputes when foundational strategy and conflict resolution aren't established&quot;" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="G4" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="H4" r:id="rId10" display="Brene Brown - Dare to Lead" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="J4" r:id="rId11" display="Core Values Definition Workshop" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="P4" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="R4" r:id="rId13" display="Don’t attempt the entrepreneurial journey solo. Numerous startups fail because they lack a robust network of supporters who can help promote their business. This includes organisations embarking on similar ventures, suppliers who can cater to startup needs, and industry veterans who have already achieved success. " xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="S4" r:id="rId14" display="Don’t attempt the entrepreneurial journey solo. Numerous startups fail because they lack a robust network of supporters who can help promote their business. This includes organisations embarking on similar ventures, suppliers who can cater to startup needs, and industry veterans who have already achieved success. " xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="T4" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="I5" r:id="rId16" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="J5" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="K5" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="L5" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
+    <hyperlink ref="N5" r:id="rId20" xr:uid="{00000000-0004-0000-0500-000014000000}"/>
+    <hyperlink ref="P5" r:id="rId21" xr:uid="{00000000-0004-0000-0500-000015000000}"/>
+    <hyperlink ref="R5" r:id="rId22" display="In retrospect, 51.3% of the surveyed founders thought they were adequately prepared when they launched their startup. No wonder so many advised better planning. “Research, research, research. Research your market,” said one founder. To that we offer an addendum: turn all that research into a business plan." xr:uid="{00000000-0004-0000-0500-000016000000}"/>
+    <hyperlink ref="T5" r:id="rId23" display="suppose the startup owner fails to draw up a comprehensive business plan or build a business model that seems sustainable over the long run. In that case, the startup might lose money, encounter operational issues, and run into legal problems." xr:uid="{00000000-0004-0000-0500-000017000000}"/>
+    <hyperlink ref="U5" r:id="rId24" xr:uid="{00000000-0004-0000-0500-000018000000}"/>
+    <hyperlink ref="H6" r:id="rId25" xr:uid="{00000000-0004-0000-0500-000019000000}"/>
+    <hyperlink ref="I6" r:id="rId26" xr:uid="{00000000-0004-0000-0500-00001A000000}"/>
+    <hyperlink ref="J6" r:id="rId27" display="Jobs To Be Done Framework" xr:uid="{00000000-0004-0000-0500-00001B000000}"/>
+    <hyperlink ref="K6" r:id="rId28" xr:uid="{00000000-0004-0000-0500-00001C000000}"/>
+    <hyperlink ref="P6" r:id="rId29" xr:uid="{00000000-0004-0000-0500-00001D000000}"/>
+    <hyperlink ref="R6" r:id="rId30" display="&quot;Overwhelming Competition - Inability to keep pace with innovators or differentiate&quot;" xr:uid="{00000000-0004-0000-0500-00001E000000}"/>
+    <hyperlink ref="S6" r:id="rId31" display="Emulation may be the sincerest form of flattery, but it does not always translate into good business. Understanding the existing market players is critical if you intend to capitalise on being a fast follower. However, it’s important to note that many start-ups that merely follow trends often fail." xr:uid="{00000000-0004-0000-0500-00001F000000}"/>
+    <hyperlink ref="G7" r:id="rId32" xr:uid="{00000000-0004-0000-0500-000020000000}"/>
+    <hyperlink ref="H7" r:id="rId33" xr:uid="{00000000-0004-0000-0500-000021000000}"/>
+    <hyperlink ref="I7" r:id="rId34" xr:uid="{00000000-0004-0000-0500-000022000000}"/>
+    <hyperlink ref="P7" r:id="rId35" xr:uid="{00000000-0004-0000-0500-000023000000}"/>
+    <hyperlink ref="R7" r:id="rId36" display="&quot;Poor Tax and Statutory Compliance - Missing taxes, superannuation, and insurance obligations damages creditworthiness and business value&quot;" xr:uid="{00000000-0004-0000-0500-000024000000}"/>
+    <hyperlink ref="G8" r:id="rId37" xr:uid="{00000000-0004-0000-0500-000025000000}"/>
+    <hyperlink ref="H8" r:id="rId38" xr:uid="{00000000-0004-0000-0500-000026000000}"/>
+    <hyperlink ref="I8" r:id="rId39" xr:uid="{00000000-0004-0000-0500-000027000000}"/>
+    <hyperlink ref="P8" r:id="rId40" display="Proof of Concept and Validation are significant factors that VCs consider when assessing startups. VCs want to see evidence that the startup's product or service has been tested or proven in the market. This validation shows that there is demand for the offering and reduces the risk of failure. It can be demonstrated through metrics such as user adoption, revenue growth, or partnerships." xr:uid="{00000000-0004-0000-0500-000028000000}"/>
+    <hyperlink ref="R8" r:id="rId41" display="Startups waste months building features nobody wants. An MVP should test your riskiest assumption with minimum effort. - Ash Maurya" xr:uid="{00000000-0004-0000-0500-000029000000}"/>
+    <hyperlink ref="I9" r:id="rId42" xr:uid="{00000000-0004-0000-0500-00002A000000}"/>
+    <hyperlink ref="J9" r:id="rId43" xr:uid="{00000000-0004-0000-0500-00002B000000}"/>
+    <hyperlink ref="N9" r:id="rId44" xr:uid="{00000000-0004-0000-0500-00002D000000}"/>
+    <hyperlink ref="P9" r:id="rId45" xr:uid="{00000000-0004-0000-0500-00002E000000}"/>
+    <hyperlink ref="R9" r:id="rId46" xr:uid="{00000000-0004-0000-0500-00002F000000}"/>
+    <hyperlink ref="S9" r:id="rId47" display=" if no market exists for the startup’s product or service, even the most creative and well-executed marketing strategy will fail. Extensive market research is crucial to ensure that there is a product-market fit." xr:uid="{00000000-0004-0000-0500-000030000000}"/>
+    <hyperlink ref="L10" r:id="rId48" xr:uid="{00000000-0004-0000-0500-000031000000}"/>
+    <hyperlink ref="P10" r:id="rId49" xr:uid="{00000000-0004-0000-0500-000034000000}"/>
+    <hyperlink ref="R10" r:id="rId50" display="&quot;Focusing on Marketing Too Little or Too Late - Underinvesting in strategic marketing or depending on single channels, limiting scalability and creating vulnerability&quot;" xr:uid="{00000000-0004-0000-0500-000035000000}"/>
+    <hyperlink ref="S10" r:id="rId51" display="&quot;Neglecting Marketing and Sales - 14% of startups fail because of poor marketing efforts — founders focus on product while ignoring customer acquisition&quot;" xr:uid="{00000000-0004-0000-0500-000036000000}"/>
+    <hyperlink ref="O11" r:id="rId52" display="Yet by neglecting to research customer needs before commencing their engineering efforts, entrepreneurs end up wasting valuable time and capital on MVPs that are likely to miss their mark. These are false starts." xr:uid="{00000000-0004-0000-0500-000037000000}"/>
+    <hyperlink ref="P11" r:id="rId53" xr:uid="{00000000-0004-0000-0500-000038000000}"/>
+    <hyperlink ref="R11" r:id="rId54" xr:uid="{00000000-0004-0000-0500-000039000000}"/>
+    <hyperlink ref="S11" r:id="rId55" xr:uid="{00000000-0004-0000-0500-00003A000000}"/>
+    <hyperlink ref="T11" r:id="rId56" xr:uid="{00000000-0004-0000-0500-00003B000000}"/>
+    <hyperlink ref="P12" r:id="rId57" xr:uid="{00000000-0004-0000-0500-00003C000000}"/>
+    <hyperlink ref="R12" r:id="rId58" xr:uid="{00000000-0004-0000-0500-00003D000000}"/>
+    <hyperlink ref="S12" r:id="rId59" xr:uid="{00000000-0004-0000-0500-00003E000000}"/>
+    <hyperlink ref="T12" r:id="rId60" xr:uid="{00000000-0004-0000-0500-00003F000000}"/>
+    <hyperlink ref="U12" r:id="rId61" xr:uid="{00000000-0004-0000-0500-000040000000}"/>
+    <hyperlink ref="P13" r:id="rId62" xr:uid="{00000000-0004-0000-0500-000041000000}"/>
+    <hyperlink ref="R13" r:id="rId63" xr:uid="{00000000-0004-0000-0500-000042000000}"/>
+    <hyperlink ref="T13" r:id="rId64" xr:uid="{00000000-0004-0000-0500-000043000000}"/>
+    <hyperlink ref="U13" r:id="rId65" xr:uid="{00000000-0004-0000-0500-000044000000}"/>
+    <hyperlink ref="O14" r:id="rId66" xr:uid="{00000000-0004-0000-0500-000045000000}"/>
+    <hyperlink ref="P14" r:id="rId67" xr:uid="{00000000-0004-0000-0500-000046000000}"/>
+    <hyperlink ref="R14" r:id="rId68" xr:uid="{00000000-0004-0000-0500-000047000000}"/>
+    <hyperlink ref="S14" r:id="rId69" xr:uid="{00000000-0004-0000-0500-000048000000}"/>
+    <hyperlink ref="T14" r:id="rId70" display="Obsess over cash flow projections and monitor burn rate. Start small and scale slowly in conjunction with validated customer demand. Consider starting a side hustle income stream to self-fund your startup." xr:uid="{00000000-0004-0000-0500-000049000000}"/>
+    <hyperlink ref="P15" r:id="rId71" xr:uid="{00000000-0004-0000-0500-00004A000000}"/>
+    <hyperlink ref="R15" r:id="rId72" xr:uid="{00000000-0004-0000-0500-00004B000000}"/>
+    <hyperlink ref="S15" r:id="rId73" xr:uid="{00000000-0004-0000-0500-00004C000000}"/>
+    <hyperlink ref="P16" r:id="rId74" xr:uid="{00000000-0004-0000-0500-00004D000000}"/>
+    <hyperlink ref="R16" r:id="rId75" display="While some mistakes can be attributed to sheer bad luck or external factors, most of them are caused by repeated errors on the part of the business owner. Failing to recognize patterns in one's missteps and make the needed adjustments can lead to a lack of growth or even closure." xr:uid="{00000000-0004-0000-0500-00004E000000}"/>
+    <hyperlink ref="P17" r:id="rId76" xr:uid="{00000000-0004-0000-0500-00004F000000}"/>
+    <hyperlink ref="P18" r:id="rId77" xr:uid="{00000000-0004-0000-0500-000050000000}"/>
+    <hyperlink ref="R18" r:id="rId78" xr:uid="{00000000-0004-0000-0500-000051000000}"/>
+    <hyperlink ref="S18" r:id="rId79" xr:uid="{00000000-0004-0000-0500-000052000000}"/>
+    <hyperlink ref="T18" r:id="rId80" xr:uid="{00000000-0004-0000-0500-000053000000}"/>
+    <hyperlink ref="P19" r:id="rId81" xr:uid="{00000000-0004-0000-0500-000054000000}"/>
+    <hyperlink ref="R19" r:id="rId82" display="Unforeseen situations occur, market trends change and aggressive competitors can pop up out of nowhere. Consequently, you may need to change course quickly at one point or another." xr:uid="{00000000-0004-0000-0500-000055000000}"/>
+    <hyperlink ref="S19" r:id="rId83" xr:uid="{00000000-0004-0000-0500-000056000000}"/>
+    <hyperlink ref="T19" r:id="rId84" xr:uid="{00000000-0004-0000-0500-000057000000}"/>
+    <hyperlink ref="P20" r:id="rId85" xr:uid="{00000000-0004-0000-0500-000058000000}"/>
+    <hyperlink ref="R20" r:id="rId86" display="Human capital is essential for startups to scale effectively and efficiently. Having the right people at the right time can greatly enhance a startup’s ability to navigate the complexities of expanding markets, evolving customer demands, and increasingly intricate operations." xr:uid="{00000000-0004-0000-0500-000059000000}"/>
+    <hyperlink ref="P21" r:id="rId87" xr:uid="{00000000-0004-0000-0500-00005A000000}"/>
+    <hyperlink ref="P22" r:id="rId88" xr:uid="{00000000-0004-0000-0500-00005B000000}"/>
+    <hyperlink ref="O23" r:id="rId89" xr:uid="{00000000-0004-0000-0500-00005C000000}"/>
+    <hyperlink ref="P23" r:id="rId90" xr:uid="{00000000-0004-0000-0500-00005D000000}"/>
+    <hyperlink ref="T23" r:id="rId91" xr:uid="{00000000-0004-0000-0500-00005E000000}"/>
+    <hyperlink ref="P24" r:id="rId92" xr:uid="{00000000-0004-0000-0500-00005F000000}"/>
+    <hyperlink ref="T24" r:id="rId93" xr:uid="{00000000-0004-0000-0500-000060000000}"/>
+    <hyperlink ref="O25" r:id="rId94" xr:uid="{00000000-0004-0000-0500-000061000000}"/>
+    <hyperlink ref="P25" r:id="rId95" xr:uid="{00000000-0004-0000-0500-000062000000}"/>
+    <hyperlink ref="R25" r:id="rId96" xr:uid="{00000000-0004-0000-0500-000063000000}"/>
+    <hyperlink ref="P26" r:id="rId97" xr:uid="{00000000-0004-0000-0500-000064000000}"/>
+    <hyperlink ref="R26" r:id="rId98" xr:uid="{00000000-0004-0000-0500-000065000000}"/>
+    <hyperlink ref="S26" r:id="rId99" xr:uid="{00000000-0004-0000-0500-000066000000}"/>
+    <hyperlink ref="G27" r:id="rId100" xr:uid="{00000000-0004-0000-0500-000067000000}"/>
+    <hyperlink ref="H27" r:id="rId101" display="RACI Matrix" xr:uid="{00000000-0004-0000-0500-000068000000}"/>
+    <hyperlink ref="I27" r:id="rId102" display="RAPID Decision Framework" xr:uid="{00000000-0004-0000-0500-000069000000}"/>
+    <hyperlink ref="P27" r:id="rId103" xr:uid="{00000000-0004-0000-0500-00006A000000}"/>
+    <hyperlink ref="R27" r:id="rId104" display="&quot;Misaligned Co-Founder Expectations - Unspoken assumptions create partnership breakdown. 24% of co-founder relationships dissolve within four years&quot;" xr:uid="{00000000-0004-0000-0500-00006B000000}"/>
+    <hyperlink ref="S27" r:id="rId105" display="As Dima Maslennikov notes in his recent Entrepreneur.com article on co-founder alignment, misaligned expectations and unspoken assumptions are among the top reasons partnerships break down. His research shows that 24% of co-founder relationships dissolve within four years, often because initial commitment levels were mismatched from day one." xr:uid="{00000000-0004-0000-0500-00006C000000}"/>
+    <hyperlink ref="F28" r:id="rId106" xr:uid="{00000000-0004-0000-0500-00006D000000}"/>
+    <hyperlink ref="J28" r:id="rId107" xr:uid="{00000000-0004-0000-0500-00006F000000}"/>
+    <hyperlink ref="P28" r:id="rId108" xr:uid="{00000000-0004-0000-0500-000070000000}"/>
+    <hyperlink ref="R28" r:id="rId109" xr:uid="{00000000-0004-0000-0500-000071000000}"/>
+    <hyperlink ref="S28" r:id="rId110" display="&quot;Missing taxes, superannuation, and insurance obligations damages creditworthiness and business value&quot;" xr:uid="{00000000-0004-0000-0500-000072000000}"/>
+    <hyperlink ref="G29" r:id="rId111" xr:uid="{00000000-0004-0000-0500-000073000000}"/>
+    <hyperlink ref="H29" r:id="rId112" xr:uid="{00000000-0004-0000-0500-000074000000}"/>
+    <hyperlink ref="I29" r:id="rId113" xr:uid="{00000000-0004-0000-0500-000075000000}"/>
+    <hyperlink ref="J29" r:id="rId114" xr:uid="{00000000-0004-0000-0500-000076000000}"/>
+    <hyperlink ref="O29" r:id="rId115" xr:uid="{00000000-0004-0000-0500-000077000000}"/>
+    <hyperlink ref="P29" r:id="rId116" xr:uid="{00000000-0004-0000-0500-000078000000}"/>
+    <hyperlink ref="R29" r:id="rId117" display="&quot;Creating vs Satisfying Demand - It's easier to satisfy an existing need than create demand; realistic projections of target audience are essential&quot;" xr:uid="{00000000-0004-0000-0500-000079000000}"/>
+    <hyperlink ref="S29" r:id="rId118" display="&quot;False Positives - Founders misinterpret early adopter enthusiasm as mainstream demand, then discover later customers have different needs&quot;" xr:uid="{00000000-0004-0000-0500-00007A000000}"/>
+    <hyperlink ref="T29" r:id="rId119" display="you should regularly assess how your startup solves customer problems and determine whether your pricing adequately covers any costs associated with providing a service or product." xr:uid="{00000000-0004-0000-0500-00007B000000}"/>
+    <hyperlink ref="G30" r:id="rId120" xr:uid="{00000000-0004-0000-0500-00007C000000}"/>
+    <hyperlink ref="H30" r:id="rId121" xr:uid="{00000000-0004-0000-0500-00007D000000}"/>
+    <hyperlink ref="I30" r:id="rId122" xr:uid="{00000000-0004-0000-0500-00007E000000}"/>
+    <hyperlink ref="P30" r:id="rId123" xr:uid="{00000000-0004-0000-0500-00007F000000}"/>
+    <hyperlink ref="R30" r:id="rId124" display="&quot;Marketing Problems (56%) - Lack of product-market fit; insufficient validation of assumptions before resource investment. Don't invest a lot of time and resources before you are confident people want what you are offering.&quot;" xr:uid="{00000000-0004-0000-0500-000080000000}"/>
+    <hyperlink ref="S30" r:id="rId125" display="Early-stage startups need to spend up to 3x longer validating their target markets than their founders anticipate. One of the aims of the more extended market validation period is to prevent cash flow issues from running the project into the ground before the startup has the chance to determine the market-product fit." xr:uid="{00000000-0004-0000-0500-000081000000}"/>
+    <hyperlink ref="T30" r:id="rId126" xr:uid="{00000000-0004-0000-0500-000082000000}"/>
+    <hyperlink ref="H31" r:id="rId127" xr:uid="{00000000-0004-0000-0500-000084000000}"/>
+    <hyperlink ref="R31" r:id="rId128" display="&quot;Competitive Blindness - Entrepreneurs who skip competitive analysis and user testing of rival products miss critical insights about market strengths and weaknesses&quot;" xr:uid="{00000000-0004-0000-0500-000087000000}"/>
+    <hyperlink ref="G31" r:id="rId129" xr:uid="{00000000-0004-0000-0500-000089000000}"/>
+    <hyperlink ref="J31" r:id="rId130" xr:uid="{00000000-0004-0000-0500-00008A000000}"/>
+    <hyperlink ref="P31" r:id="rId131" xr:uid="{00000000-0004-0000-0500-00008B000000}"/>
+    <hyperlink ref="S31" r:id="rId132" display="&quot;42% of startups fail from no market need. Surveys lie - people say they'll buy, then don't. Test with behaviour (pre-orders, pilots), not surveys.&quot; - CB Insights" xr:uid="{00000000-0004-0000-0500-00008C000000}"/>
+    <hyperlink ref="T31" r:id="rId133" display="Conducting market surveys, engaging with potential customers, identifying competitors, and exploring untapped market opportunities are essential. These actions significantly reduce the risk of a startup’s efforts being in vain, ensuring a more informed and strategic approach to market entry. " xr:uid="{00000000-0004-0000-0500-00008D000000}"/>
+    <hyperlink ref="U31" r:id="rId134" xr:uid="{00000000-0004-0000-0500-00008E000000}"/>
+    <hyperlink ref="G32" r:id="rId135" xr:uid="{00000000-0004-0000-0500-00008F000000}"/>
+    <hyperlink ref="H32" r:id="rId136" xr:uid="{00000000-0004-0000-0500-000090000000}"/>
+    <hyperlink ref="N32" r:id="rId137" xr:uid="{00000000-0004-0000-0500-000091000000}"/>
+    <hyperlink ref="U32" r:id="rId138" location=":~:text=changes%20can%20reveal%20surprising%20and,you%20might've%20never%20expected.&amp;text=Even%20the%20best%20qualitative%20theory,a%20greater%20height%20through%20experimentation." xr:uid="{00000000-0004-0000-0500-000093000000}"/>
+    <hyperlink ref="G33" r:id="rId139" xr:uid="{00000000-0004-0000-0500-000094000000}"/>
+    <hyperlink ref="H33" r:id="rId140" xr:uid="{00000000-0004-0000-0500-000095000000}"/>
+    <hyperlink ref="I33" r:id="rId141" xr:uid="{00000000-0004-0000-0500-000096000000}"/>
+    <hyperlink ref="J33" r:id="rId142" xr:uid="{00000000-0004-0000-0500-000097000000}"/>
+    <hyperlink ref="N33" r:id="rId143" xr:uid="{00000000-0004-0000-0500-000098000000}"/>
+    <hyperlink ref="P33" r:id="rId144" xr:uid="{00000000-0004-0000-0500-000099000000}"/>
+    <hyperlink ref="R33" r:id="rId145" xr:uid="{00000000-0004-0000-0500-00009A000000}"/>
+    <hyperlink ref="T33" r:id="rId146" xr:uid="{00000000-0004-0000-0500-00009B000000}"/>
+    <hyperlink ref="U33" r:id="rId147" xr:uid="{00000000-0004-0000-0500-00009C000000}"/>
+    <hyperlink ref="G34" r:id="rId148" xr:uid="{00000000-0004-0000-0500-00009D000000}"/>
+    <hyperlink ref="H34" r:id="rId149" xr:uid="{00000000-0004-0000-0500-00009E000000}"/>
+    <hyperlink ref="I34" r:id="rId150" display="Pilot Program Framework" xr:uid="{00000000-0004-0000-0500-00009F000000}"/>
+    <hyperlink ref="P34" r:id="rId151" xr:uid="{00000000-0004-0000-0500-0000A0000000}"/>
+    <hyperlink ref="R34" r:id="rId152" display="&quot;Research-Free Launch - Launching without thorough market research is a recipe for financial loss; demand validation is crucial before investment&quot;" xr:uid="{00000000-0004-0000-0500-0000A1000000}"/>
+    <hyperlink ref="G35" r:id="rId153" xr:uid="{00000000-0004-0000-0500-0000A2000000}"/>
+    <hyperlink ref="H35" r:id="rId154" xr:uid="{00000000-0004-0000-0500-0000A3000000}"/>
+    <hyperlink ref="I35" r:id="rId155" display="Activation Metric Examples" xr:uid="{00000000-0004-0000-0500-0000A4000000}"/>
+    <hyperlink ref="J35" r:id="rId156" xr:uid="{00000000-0004-0000-0500-0000A5000000}"/>
+    <hyperlink ref="P35" r:id="rId157" xr:uid="{00000000-0004-0000-0500-0000A6000000}"/>
+    <hyperlink ref="R35" r:id="rId158" xr:uid="{00000000-0004-0000-0500-0000A7000000}"/>
+    <hyperlink ref="T35" r:id="rId159" display="&quot;DAU/MAU ratio of 20%+ is good for most consumer products. If it's dropping, you have an engagement problem before you have a growth problem.&quot; - Lenny Rachitsky" xr:uid="{00000000-0004-0000-0500-0000A8000000}"/>
+    <hyperlink ref="G36" r:id="rId160" display="Pre-Launch Marketing Tactics" xr:uid="{00000000-0004-0000-0500-0000A9000000}"/>
+    <hyperlink ref="H36" r:id="rId161" xr:uid="{00000000-0004-0000-0500-0000AA000000}"/>
+    <hyperlink ref="I36" r:id="rId162" xr:uid="{00000000-0004-0000-0500-0000AB000000}"/>
+    <hyperlink ref="P36" r:id="rId163" xr:uid="{00000000-0004-0000-0500-0000AC000000}"/>
+    <hyperlink ref="R36" r:id="rId164" display="&quot;Poor Marketing Execution - 14% of startups fail because of poor marketing efforts; founders focus all energy on product development and neglect critical marketing activities&quot;" xr:uid="{00000000-0004-0000-0500-0000AD000000}"/>
+    <hyperlink ref="T36" r:id="rId165" xr:uid="{00000000-0004-0000-0500-0000AE000000}"/>
+    <hyperlink ref="P37" r:id="rId166" xr:uid="{00000000-0004-0000-0500-0000AF000000}"/>
+    <hyperlink ref="R37" r:id="rId167" xr:uid="{00000000-0004-0000-0500-0000B0000000}"/>
+    <hyperlink ref="S37" r:id="rId168" xr:uid="{00000000-0004-0000-0500-0000B1000000}"/>
+    <hyperlink ref="T37" r:id="rId169" xr:uid="{00000000-0004-0000-0500-0000B2000000}"/>
+    <hyperlink ref="P38" r:id="rId170" xr:uid="{00000000-0004-0000-0500-0000B3000000}"/>
+    <hyperlink ref="R38" r:id="rId171" xr:uid="{00000000-0004-0000-0500-0000B4000000}"/>
+    <hyperlink ref="S38" r:id="rId172" xr:uid="{00000000-0004-0000-0500-0000B5000000}"/>
+    <hyperlink ref="T38" r:id="rId173" xr:uid="{00000000-0004-0000-0500-0000B6000000}"/>
+    <hyperlink ref="P39" r:id="rId174" xr:uid="{00000000-0004-0000-0500-0000B7000000}"/>
+    <hyperlink ref="R39" r:id="rId175" xr:uid="{00000000-0004-0000-0500-0000B8000000}"/>
+    <hyperlink ref="P40" r:id="rId176" xr:uid="{00000000-0004-0000-0500-0000B9000000}"/>
+    <hyperlink ref="R40" r:id="rId177" xr:uid="{00000000-0004-0000-0500-0000BA000000}"/>
+    <hyperlink ref="T40" r:id="rId178" xr:uid="{00000000-0004-0000-0500-0000BB000000}"/>
+    <hyperlink ref="P41" r:id="rId179" xr:uid="{00000000-0004-0000-0500-0000BC000000}"/>
+    <hyperlink ref="R41" r:id="rId180" xr:uid="{00000000-0004-0000-0500-0000BD000000}"/>
+    <hyperlink ref="S41" r:id="rId181" xr:uid="{00000000-0004-0000-0500-0000BE000000}"/>
+    <hyperlink ref="T41" r:id="rId182" xr:uid="{00000000-0004-0000-0500-0000BF000000}"/>
+    <hyperlink ref="P42" r:id="rId183" xr:uid="{00000000-0004-0000-0500-0000C0000000}"/>
+    <hyperlink ref="R42" r:id="rId184" xr:uid="{00000000-0004-0000-0500-0000C1000000}"/>
+    <hyperlink ref="T42" r:id="rId185" xr:uid="{00000000-0004-0000-0500-0000C2000000}"/>
+    <hyperlink ref="U42" r:id="rId186" xr:uid="{00000000-0004-0000-0500-0000C3000000}"/>
+    <hyperlink ref="G43" r:id="rId187" xr:uid="{00000000-0004-0000-0500-0000C4000000}"/>
+    <hyperlink ref="H43" r:id="rId188" xr:uid="{00000000-0004-0000-0500-0000C5000000}"/>
+    <hyperlink ref="I43" r:id="rId189" xr:uid="{00000000-0004-0000-0500-0000C6000000}"/>
+    <hyperlink ref="P43" r:id="rId190" xr:uid="{00000000-0004-0000-0500-0000C7000000}"/>
+    <hyperlink ref="R43" r:id="rId191" xr:uid="{00000000-0004-0000-0500-0000C8000000}"/>
+    <hyperlink ref="T43" r:id="rId192" xr:uid="{00000000-0004-0000-0500-0000C9000000}"/>
+    <hyperlink ref="U43" r:id="rId193" xr:uid="{00000000-0004-0000-0500-0000CA000000}"/>
+    <hyperlink ref="P44" r:id="rId194" xr:uid="{00000000-0004-0000-0500-0000CB000000}"/>
+    <hyperlink ref="R44" r:id="rId195" xr:uid="{00000000-0004-0000-0500-0000CC000000}"/>
+    <hyperlink ref="S44" r:id="rId196" xr:uid="{00000000-0004-0000-0500-0000CD000000}"/>
+    <hyperlink ref="T44" r:id="rId197" xr:uid="{00000000-0004-0000-0500-0000CE000000}"/>
+    <hyperlink ref="U44" r:id="rId198" xr:uid="{00000000-0004-0000-0500-0000CF000000}"/>
+    <hyperlink ref="P45" r:id="rId199" xr:uid="{00000000-0004-0000-0500-0000D0000000}"/>
+    <hyperlink ref="R45" r:id="rId200" xr:uid="{00000000-0004-0000-0500-0000D1000000}"/>
+    <hyperlink ref="S45" r:id="rId201" xr:uid="{00000000-0004-0000-0500-0000D2000000}"/>
+    <hyperlink ref="T45" r:id="rId202" xr:uid="{00000000-0004-0000-0500-0000D3000000}"/>
+    <hyperlink ref="P46" r:id="rId203" xr:uid="{00000000-0004-0000-0500-0000D4000000}"/>
+    <hyperlink ref="R46" r:id="rId204" xr:uid="{00000000-0004-0000-0500-0000D5000000}"/>
+    <hyperlink ref="S46" r:id="rId205" xr:uid="{00000000-0004-0000-0500-0000D6000000}"/>
+    <hyperlink ref="P47" r:id="rId206" xr:uid="{00000000-0004-0000-0500-0000D7000000}"/>
+    <hyperlink ref="P48" r:id="rId207" xr:uid="{00000000-0004-0000-0500-0000D8000000}"/>
+    <hyperlink ref="P49" r:id="rId208" xr:uid="{00000000-0004-0000-0500-0000D9000000}"/>
+    <hyperlink ref="P50" r:id="rId209" xr:uid="{00000000-0004-0000-0500-0000DA000000}"/>
+    <hyperlink ref="T50" r:id="rId210" xr:uid="{00000000-0004-0000-0500-0000DB000000}"/>
+    <hyperlink ref="P51" r:id="rId211" xr:uid="{00000000-0004-0000-0500-0000DC000000}"/>
+    <hyperlink ref="R51" r:id="rId212" xr:uid="{00000000-0004-0000-0500-0000DD000000}"/>
+    <hyperlink ref="T51" r:id="rId213" xr:uid="{00000000-0004-0000-0500-0000DE000000}"/>
+    <hyperlink ref="P52" r:id="rId214" xr:uid="{00000000-0004-0000-0500-0000DF000000}"/>
+    <hyperlink ref="R52" r:id="rId215" xr:uid="{00000000-0004-0000-0500-0000E0000000}"/>
+    <hyperlink ref="T52" r:id="rId216" xr:uid="{00000000-0004-0000-0500-0000E1000000}"/>
+    <hyperlink ref="G53" r:id="rId217" xr:uid="{00000000-0004-0000-0500-0000E2000000}"/>
+    <hyperlink ref="H53" r:id="rId218" xr:uid="{00000000-0004-0000-0500-0000E3000000}"/>
+    <hyperlink ref="P53" r:id="rId219" xr:uid="{00000000-0004-0000-0500-0000E4000000}"/>
+    <hyperlink ref="R53" r:id="rId220" display="&quot;Founder Quality - VCs look for founders with resilience, passion, and experience leading start-up teams — the right stuff matters more than the idea&quot;" xr:uid="{00000000-0004-0000-0500-0000E5000000}"/>
+    <hyperlink ref="S53" r:id="rId221" xr:uid="{00000000-0004-0000-0500-0000E6000000}"/>
+    <hyperlink ref="T53" r:id="rId222" xr:uid="{00000000-0004-0000-0500-0000E7000000}"/>
+    <hyperlink ref="U53" r:id="rId223" xr:uid="{00000000-0004-0000-0500-0000E8000000}"/>
+    <hyperlink ref="H54" r:id="rId224" xr:uid="{00000000-0004-0000-0500-0000EB000000}"/>
+    <hyperlink ref="I54" r:id="rId225" xr:uid="{00000000-0004-0000-0500-0000EC000000}"/>
+    <hyperlink ref="P54" r:id="rId226" xr:uid="{00000000-0004-0000-0500-0000ED000000}"/>
+    <hyperlink ref="R54" r:id="rId227" display="&quot;Governance Problems - Lack of foundational legal structure, compliance oversight, and board governance creates operational vulnerability and limits investment readiness&quot;" xr:uid="{00000000-0004-0000-0500-0000EE000000}"/>
+    <hyperlink ref="G55" r:id="rId228" xr:uid="{00000000-0004-0000-0500-0000EF000000}"/>
+    <hyperlink ref="P55" r:id="rId229" xr:uid="{00000000-0004-0000-0500-0000F0000000}"/>
+    <hyperlink ref="R55" r:id="rId230" display="&quot;Founder Quality - VCs look for founders with resilience, passion, and experience leading start-up teams   —   the right stuff matters more than the idea&quot;" xr:uid="{00000000-0004-0000-0500-0000F1000000}"/>
+    <hyperlink ref="G56" r:id="rId231" xr:uid="{00000000-0004-0000-0500-0000F2000000}"/>
+    <hyperlink ref="H56" r:id="rId232" xr:uid="{00000000-0004-0000-0500-0000F3000000}"/>
+    <hyperlink ref="P56" r:id="rId233" xr:uid="{00000000-0004-0000-0500-0000F4000000}"/>
+    <hyperlink ref="R56" r:id="rId234" xr:uid="{00000000-0004-0000-0500-0000F5000000}"/>
+    <hyperlink ref="S56" r:id="rId235" display="To expect communication naturally evolves with growth, for instance, is a false assumption many startup founders make. It’s obviously a lot easier to communicate changes and progress to a few other people, versus 10, 50 or even 1000 other people." xr:uid="{00000000-0004-0000-0500-0000F6000000}"/>
+    <hyperlink ref="T56" r:id="rId236" display="try to keep up with trends in your industry and be open to feedback that can help you improve the overall quality of your service or product." xr:uid="{00000000-0004-0000-0500-0000F7000000}"/>
+    <hyperlink ref="U56" r:id="rId237" xr:uid="{00000000-0004-0000-0500-0000F8000000}"/>
+    <hyperlink ref="G57" r:id="rId238" xr:uid="{00000000-0004-0000-0500-0000F9000000}"/>
+    <hyperlink ref="P57" r:id="rId239" xr:uid="{00000000-0004-0000-0500-0000FA000000}"/>
+    <hyperlink ref="R57" r:id="rId240" display="&quot;Market Adaptation Failure - Whether it's consumer preference shifts or black swan events like coronavirus, startups must adapt quickly to survive&quot;" xr:uid="{00000000-0004-0000-0500-0000FB000000}"/>
+    <hyperlink ref="T57" r:id="rId241" xr:uid="{00000000-0004-0000-0500-0000FC000000}"/>
+    <hyperlink ref="G58" r:id="rId242" xr:uid="{00000000-0004-0000-0500-0000FD000000}"/>
+    <hyperlink ref="H58" r:id="rId243" xr:uid="{00000000-0004-0000-0500-0000FE000000}"/>
+    <hyperlink ref="P58" r:id="rId244" xr:uid="{00000000-0004-0000-0500-0000FF000000}"/>
+    <hyperlink ref="R58" r:id="rId245" display="&quot;Pivot Necessity - 75% of startups change their initial ideas as the market landscape shifts; rigidly clinging to original plans guarantees failure&quot;" xr:uid="{00000000-0004-0000-0500-000000010000}"/>
+    <hyperlink ref="S58" r:id="rId246" xr:uid="{00000000-0004-0000-0500-000001010000}"/>
+    <hyperlink ref="T58" r:id="rId247" xr:uid="{00000000-0004-0000-0500-000002010000}"/>
+    <hyperlink ref="G59" r:id="rId248" xr:uid="{00000000-0004-0000-0500-000003010000}"/>
+    <hyperlink ref="H59" r:id="rId249" xr:uid="{00000000-0004-0000-0500-000004010000}"/>
+    <hyperlink ref="P59" r:id="rId250" xr:uid="{00000000-0004-0000-0500-000005010000}"/>
+    <hyperlink ref="R59" r:id="rId251" display="&quot;Customer-Led Development - We let the thousands decide what the millions will do — early customer feedback guides mass market decisions&quot;" xr:uid="{00000000-0004-0000-0500-000006010000}"/>
+    <hyperlink ref="T59" r:id="rId252" xr:uid="{00000000-0004-0000-0500-000007010000}"/>
+    <hyperlink ref="G60" r:id="rId253" xr:uid="{00000000-0004-0000-0500-000008010000}"/>
+    <hyperlink ref="H60" r:id="rId254" xr:uid="{00000000-0004-0000-0500-000009010000}"/>
+    <hyperlink ref="P60" r:id="rId255" xr:uid="{00000000-0004-0000-0500-00000A010000}"/>
+    <hyperlink ref="R60" r:id="rId256" display="&quot;Customer-Led Development - We let the thousands decide what the millions will do   —   early customer feedback guides mass market decisions&quot;" xr:uid="{00000000-0004-0000-0500-00000B010000}"/>
+    <hyperlink ref="T60" r:id="rId257" xr:uid="{00000000-0004-0000-0500-00000C010000}"/>
+    <hyperlink ref="J61" r:id="rId258" xr:uid="{00000000-0004-0000-0500-00000D010000}"/>
+    <hyperlink ref="K61" r:id="rId259" xr:uid="{00000000-0004-0000-0500-00000E010000}"/>
+    <hyperlink ref="L61" r:id="rId260" xr:uid="{00000000-0004-0000-0500-00000F010000}"/>
+    <hyperlink ref="G62" r:id="rId261" xr:uid="{00000000-0004-0000-0500-000013010000}"/>
+    <hyperlink ref="H62" r:id="rId262" xr:uid="{00000000-0004-0000-0500-000014010000}"/>
+    <hyperlink ref="P62" r:id="rId263" xr:uid="{00000000-0004-0000-0500-000015010000}"/>
+    <hyperlink ref="R62" r:id="rId264" xr:uid="{00000000-0004-0000-0500-000016010000}"/>
+    <hyperlink ref="S62" r:id="rId265" xr:uid="{00000000-0004-0000-0500-000017010000}"/>
+    <hyperlink ref="T62" r:id="rId266" xr:uid="{00000000-0004-0000-0500-000018010000}"/>
+    <hyperlink ref="U62" r:id="rId267" xr:uid="{00000000-0004-0000-0500-000019010000}"/>
+    <hyperlink ref="G61" r:id="rId268" xr:uid="{00000000-0004-0000-0500-00001A010000}"/>
+    <hyperlink ref="H61" r:id="rId269" xr:uid="{00000000-0004-0000-0500-00001B010000}"/>
+    <hyperlink ref="I61" r:id="rId270" xr:uid="{00000000-0004-0000-0500-00001C010000}"/>
+    <hyperlink ref="P61" r:id="rId271" xr:uid="{00000000-0004-0000-0500-00001D010000}"/>
+    <hyperlink ref="S61" r:id="rId272" display="&quot;Innovation Failure - MySpace failed to innovate, didn't track young users' rapidly changing habits, and quickly fell behind Facebook&quot;" xr:uid="{00000000-0004-0000-0500-00001E010000}"/>
+    <hyperlink ref="T61" r:id="rId273" xr:uid="{00000000-0004-0000-0500-00001F010000}"/>
+    <hyperlink ref="P63" r:id="rId274" xr:uid="{00000000-0004-0000-0500-000020010000}"/>
+    <hyperlink ref="R63" r:id="rId275" display="&quot;Insufficient Network/Allies - Lack of referral sources and industry connections limits growth acceleration and credibility&quot;" xr:uid="{00000000-0004-0000-0500-000021010000}"/>
+    <hyperlink ref="T64" r:id="rId276" display="Ensure you have a strong presence on the right social media channels and utilize them to their fullest potential." xr:uid="{00000000-0004-0000-0500-000022010000}"/>
+    <hyperlink ref="G64" r:id="rId277" xr:uid="{00000000-0004-0000-0500-000023010000}"/>
+    <hyperlink ref="H64" r:id="rId278" xr:uid="{00000000-0004-0000-0500-000024010000}"/>
+    <hyperlink ref="P64" r:id="rId279" xr:uid="{00000000-0004-0000-0500-000025010000}"/>
+    <hyperlink ref="R64" r:id="rId280" display="&quot;Customer Service Orientation (66% of sample) - Prioritized new customer acquisition over retention; focused on technological solutions rather than customer needs&quot;" xr:uid="{00000000-0004-0000-0500-000026010000}"/>
+    <hyperlink ref="G65" r:id="rId281" xr:uid="{00000000-0004-0000-0500-000027010000}"/>
+    <hyperlink ref="H65" r:id="rId282" xr:uid="{00000000-0004-0000-0500-000028010000}"/>
+    <hyperlink ref="I65" r:id="rId283" xr:uid="{00000000-0004-0000-0500-000029010000}"/>
+    <hyperlink ref="P65" r:id="rId284" xr:uid="{00000000-0004-0000-0500-00002A010000}"/>
+    <hyperlink ref="R65" r:id="rId285" display="&quot;Customer Service Orientation (66% of sample) - Prioritised new customer acquisition over retention; focused on technological solutions rather than customer needs&quot;" xr:uid="{00000000-0004-0000-0500-00002B010000}"/>
+    <hyperlink ref="P66" r:id="rId286" xr:uid="{00000000-0004-0000-0500-00002C010000}"/>
+    <hyperlink ref="R66" r:id="rId287" xr:uid="{00000000-0004-0000-0500-00002D010000}"/>
+    <hyperlink ref="S66" r:id="rId288" xr:uid="{00000000-0004-0000-0500-00002E010000}"/>
+    <hyperlink ref="T66" r:id="rId289" display="seek advice from experienced entrepreneurs who have gone through the process before, as they can provide valuable insight and feedback." xr:uid="{00000000-0004-0000-0500-00002F010000}"/>
+    <hyperlink ref="P67" r:id="rId290" xr:uid="{00000000-0004-0000-0500-000030010000}"/>
+    <hyperlink ref="R67" r:id="rId291" xr:uid="{00000000-0004-0000-0500-000031010000}"/>
+    <hyperlink ref="S67" r:id="rId292" xr:uid="{00000000-0004-0000-0500-000032010000}"/>
+    <hyperlink ref="T67" r:id="rId293" display="Analyzing your overall business performance is also important. If your business goals, product development goals, marketing iniatives, and team communications are becoming confusing or uncertain, this won’t go over well in your next pitch meeting. Investors want to see a clear vision, a clear pathway to success, and evidence that you can follow through." xr:uid="{00000000-0004-0000-0500-000033010000}"/>
+    <hyperlink ref="P68" r:id="rId294" xr:uid="{00000000-0004-0000-0500-000034010000}"/>
+    <hyperlink ref="R68" r:id="rId295" xr:uid="{00000000-0004-0000-0500-000035010000}"/>
+    <hyperlink ref="S68" r:id="rId296" xr:uid="{00000000-0004-0000-0500-000036010000}"/>
+    <hyperlink ref="P69" r:id="rId297" xr:uid="{00000000-0004-0000-0500-000037010000}"/>
+    <hyperlink ref="R69" r:id="rId298" xr:uid="{00000000-0004-0000-0500-000038010000}"/>
+    <hyperlink ref="S69" r:id="rId299" xr:uid="{00000000-0004-0000-0500-000039010000}"/>
+    <hyperlink ref="P70" r:id="rId300" xr:uid="{00000000-0004-0000-0500-00003A010000}"/>
+    <hyperlink ref="R70" r:id="rId301" xr:uid="{00000000-0004-0000-0500-00003B010000}"/>
+    <hyperlink ref="S70" r:id="rId302" xr:uid="{00000000-0004-0000-0500-00003C010000}"/>
+    <hyperlink ref="P71" r:id="rId303" xr:uid="{00000000-0004-0000-0500-00003D010000}"/>
+    <hyperlink ref="T71" r:id="rId304" xr:uid="{00000000-0004-0000-0500-00003E010000}"/>
+    <hyperlink ref="P72" r:id="rId305" xr:uid="{00000000-0004-0000-0500-00003F010000}"/>
+    <hyperlink ref="R72" r:id="rId306" xr:uid="{00000000-0004-0000-0500-000040010000}"/>
+    <hyperlink ref="T72" r:id="rId307" xr:uid="{00000000-0004-0000-0500-000041010000}"/>
+    <hyperlink ref="P73" r:id="rId308" xr:uid="{00000000-0004-0000-0500-000042010000}"/>
+    <hyperlink ref="R73" r:id="rId309" xr:uid="{00000000-0004-0000-0500-000043010000}"/>
+    <hyperlink ref="T73" r:id="rId310" display="Startups should concentrate on one core offering, perfect it, and then consider expanding. Maintaining focus and prioritizing resources on a single product or service can help startups avoid spreading themselves too thin and ensure they deliver exceptional value to their customers." xr:uid="{00000000-0004-0000-0500-000044010000}"/>
+    <hyperlink ref="P74" r:id="rId311" xr:uid="{00000000-0004-0000-0500-000045010000}"/>
+    <hyperlink ref="R74" r:id="rId312" xr:uid="{00000000-0004-0000-0500-000046010000}"/>
+    <hyperlink ref="T74" r:id="rId313" xr:uid="{00000000-0004-0000-0500-000047010000}"/>
+    <hyperlink ref="U74" r:id="rId314" xr:uid="{00000000-0004-0000-0500-000048010000}"/>
+    <hyperlink ref="P75" r:id="rId315" xr:uid="{00000000-0004-0000-0500-000049010000}"/>
+    <hyperlink ref="R75" r:id="rId316" xr:uid="{00000000-0004-0000-0500-00004A010000}"/>
+    <hyperlink ref="U75" r:id="rId317" xr:uid="{00000000-0004-0000-0500-00004B010000}"/>
+    <hyperlink ref="P76" r:id="rId318" xr:uid="{00000000-0004-0000-0500-00004C010000}"/>
+    <hyperlink ref="U76" r:id="rId319" xr:uid="{00000000-0004-0000-0500-00004D010000}"/>
+    <hyperlink ref="P77" r:id="rId320" xr:uid="{00000000-0004-0000-0500-00004E010000}"/>
+    <hyperlink ref="P78" r:id="rId321" xr:uid="{00000000-0004-0000-0500-00004F010000}"/>
+    <hyperlink ref="T78" r:id="rId322" xr:uid="{00000000-0004-0000-0500-000050010000}"/>
+    <hyperlink ref="P79" r:id="rId323" xr:uid="{00000000-0004-0000-0500-000051010000}"/>
+    <hyperlink ref="P80" r:id="rId324" xr:uid="{00000000-0004-0000-0500-000052010000}"/>
+    <hyperlink ref="P81" r:id="rId325" xr:uid="{00000000-0004-0000-0500-000053010000}"/>
+    <hyperlink ref="R81" r:id="rId326" xr:uid="{00000000-0004-0000-0500-000054010000}"/>
+    <hyperlink ref="T81" r:id="rId327" xr:uid="{00000000-0004-0000-0500-000055010000}"/>
+    <hyperlink ref="G82" r:id="rId328" xr:uid="{00000000-0004-0000-0500-000056010000}"/>
+    <hyperlink ref="H82" r:id="rId329" xr:uid="{00000000-0004-0000-0500-000057010000}"/>
+    <hyperlink ref="P82" r:id="rId330" xr:uid="{00000000-0004-0000-0500-000058010000}"/>
+    <hyperlink ref="R82" r:id="rId331" xr:uid="{00000000-0004-0000-0500-000059010000}"/>
+    <hyperlink ref="S82" r:id="rId332" xr:uid="{00000000-0004-0000-0500-00005A010000}"/>
+    <hyperlink ref="T82" r:id="rId333" xr:uid="{00000000-0004-0000-0500-00005B010000}"/>
+    <hyperlink ref="U82" r:id="rId334" xr:uid="{00000000-0004-0000-0500-00005C010000}"/>
+    <hyperlink ref="G83" r:id="rId335" xr:uid="{00000000-0004-0000-0500-00005D010000}"/>
+    <hyperlink ref="H83" r:id="rId336" xr:uid="{00000000-0004-0000-0500-00005E010000}"/>
+    <hyperlink ref="P83" r:id="rId337" xr:uid="{00000000-0004-0000-0500-00005F010000}"/>
+    <hyperlink ref="R83" r:id="rId338" display="&quot;Founder Over-Extension - I quickly became stretched too thin and lost connection with staff; the entire enterprise began to lose focus and flounder&quot;" xr:uid="{00000000-0004-0000-0500-000060010000}"/>
+    <hyperlink ref="T83" r:id="rId339" xr:uid="{00000000-0004-0000-0500-000061010000}"/>
+    <hyperlink ref="H84" r:id="rId340" xr:uid="{00000000-0004-0000-0500-000062010000}"/>
+    <hyperlink ref="I84" r:id="rId341" xr:uid="{00000000-0004-0000-0500-000063010000}"/>
+    <hyperlink ref="J84" r:id="rId342" xr:uid="{00000000-0004-0000-0500-000064010000}"/>
+    <hyperlink ref="P84" r:id="rId343" xr:uid="{00000000-0004-0000-0500-000065010000}"/>
+    <hyperlink ref="R84" r:id="rId344" display="&quot;Team Problems - 23% of startups fail from missing expertise and weak leadership. Early-stage teams lack experienced leaders who can scale operations, resulting in founder burnout and operational chaos as complexity increases.&quot;" xr:uid="{00000000-0004-0000-0500-000066010000}"/>
+    <hyperlink ref="S84" r:id="rId345" display="&quot;Insufficient Network/Allies - Lack of referral sources and industry connections limits growth acceleration and credibility&quot;" xr:uid="{00000000-0004-0000-0500-000067010000}"/>
+    <hyperlink ref="T84" r:id="rId346" display="seek advice from experienced entrepreneurs who have gone through the process before, as they can provide valuable insight and feedback." xr:uid="{00000000-0004-0000-0500-000068010000}"/>
+    <hyperlink ref="U84" r:id="rId347" xr:uid="{00000000-0004-0000-0500-000069010000}"/>
+    <hyperlink ref="G85" r:id="rId348" xr:uid="{00000000-0004-0000-0500-00006A010000}"/>
+    <hyperlink ref="H85" r:id="rId349" xr:uid="{00000000-0004-0000-0500-00006B010000}"/>
+    <hyperlink ref="P85" r:id="rId350" xr:uid="{00000000-0004-0000-0500-00006C010000}"/>
+    <hyperlink ref="R85" r:id="rId351" xr:uid="{00000000-0004-0000-0500-00006D010000}"/>
+    <hyperlink ref="S85" r:id="rId352" display="&quot;Communication Doesn't Scale Naturally - False assumption that communication evolves automatically; communicating changes to 1000 people differs fundamentally from 10&quot;" xr:uid="{00000000-0004-0000-0500-00006E010000}"/>
+    <hyperlink ref="T85" r:id="rId353" display="Analyzing your overall business performance is also important. If your business goals, product development goals, marketing iniatives, and team communications are becoming confusing or uncertain, this won’t go over well in your next pitch meeting. Investors want to see a clear vision, a clear pathway to success, and evidence that you can follow through." xr:uid="{00000000-0004-0000-0500-00006F010000}"/>
+    <hyperlink ref="U85" r:id="rId354" xr:uid="{00000000-0004-0000-0500-000070010000}"/>
+    <hyperlink ref="G86" r:id="rId355" xr:uid="{00000000-0004-0000-0500-000071010000}"/>
+    <hyperlink ref="H86" r:id="rId356" xr:uid="{00000000-0004-0000-0500-000072010000}"/>
+    <hyperlink ref="P86" r:id="rId357" xr:uid="{00000000-0004-0000-0500-000073010000}"/>
+    <hyperlink ref="R86" r:id="rId358" display="&quot;Lacking Scalable Infrastructure - Failing to systematically establish communication systems, IT redundancy, and operational procedures for growing team sise. You need to invest in your company's communication infrastructure.&quot;" xr:uid="{00000000-0004-0000-0500-000074010000}"/>
+    <hyperlink ref="G87" r:id="rId359" xr:uid="{00000000-0004-0000-0500-000075010000}"/>
+    <hyperlink ref="P87" r:id="rId360" xr:uid="{00000000-0004-0000-0500-000076010000}"/>
+    <hyperlink ref="R87" r:id="rId361" display="&quot;Over-Customising for Customers - Saying yes to every customer feature request during scale-up creates over-promising, under-delivering, and unsustainable complexity&quot;" xr:uid="{00000000-0004-0000-0500-000077010000}"/>
+    <hyperlink ref="S87" r:id="rId362" xr:uid="{00000000-0004-0000-0500-000078010000}"/>
+    <hyperlink ref="G88" r:id="rId363" xr:uid="{00000000-0004-0000-0500-000079010000}"/>
+    <hyperlink ref="H88" r:id="rId364" xr:uid="{00000000-0004-0000-0500-00007A010000}"/>
+    <hyperlink ref="P88" r:id="rId365" xr:uid="{00000000-0004-0000-0500-00007B010000}"/>
+    <hyperlink ref="R88" r:id="rId366" display="&quot;Pivot Failure - Textbook example: Blockbuster had 9,000+ stores and owned movie-rental market but failed to pivot when market shifted&quot;" xr:uid="{00000000-0004-0000-0500-00007C010000}"/>
+    <hyperlink ref="G89" r:id="rId367" xr:uid="{00000000-0004-0000-0500-00007D010000}"/>
+    <hyperlink ref="H89" r:id="rId368" xr:uid="{00000000-0004-0000-0500-00007E010000}"/>
+    <hyperlink ref="P89" r:id="rId369" xr:uid="{00000000-0004-0000-0500-00007F010000}"/>
+    <hyperlink ref="R89" r:id="rId370" display="&quot;Leadership Dysfunction - Dysfunction at the top quickly infects the entire organisation, draining morale and destroying culture&quot;" xr:uid="{00000000-0004-0000-0500-000080010000}"/>
+    <hyperlink ref="T89" r:id="rId371" xr:uid="{00000000-0004-0000-0500-000081010000}"/>
+    <hyperlink ref="U89" r:id="rId372" xr:uid="{00000000-0004-0000-0500-000082010000}"/>
+    <hyperlink ref="G90" r:id="rId373" xr:uid="{00000000-0004-0000-0500-000083010000}"/>
+    <hyperlink ref="P90" r:id="rId374" xr:uid="{00000000-0004-0000-0500-000084010000}"/>
+    <hyperlink ref="R90" r:id="rId375" xr:uid="{00000000-0004-0000-0500-000085010000}"/>
+    <hyperlink ref="S90" r:id="rId376" xr:uid="{00000000-0004-0000-0500-000086010000}"/>
+    <hyperlink ref="T90" r:id="rId377" xr:uid="{00000000-0004-0000-0500-000087010000}"/>
+    <hyperlink ref="G91" r:id="rId378" xr:uid="{00000000-0004-0000-0500-000088010000}"/>
+    <hyperlink ref="H91" r:id="rId379" xr:uid="{00000000-0004-0000-0500-000089010000}"/>
+    <hyperlink ref="P91" r:id="rId380" xr:uid="{00000000-0004-0000-0500-00008A010000}"/>
+    <hyperlink ref="R91" r:id="rId381" display="Startups fail by spreading too thin across multiple markets/channels simultaneously. Dominate one market before expanding to next. - CB Insights" xr:uid="{00000000-0004-0000-0500-00008B010000}"/>
+    <hyperlink ref="S91" r:id="rId382" display="&quot;Offering Too Many Services - Trying to serve all markets increases operational complexity and diverts from core purpose&quot;" xr:uid="{00000000-0004-0000-0500-00008C010000}"/>
+    <hyperlink ref="T91" r:id="rId383" display="Startups should concentrate on one core offering, perfect it, and then consider expanding. Maintaining focus and prioritizing resources on a single product or service can help startups avoid spreading themselves too thin and ensure they deliver exceptional value to their customers." xr:uid="{00000000-0004-0000-0500-00008D010000}"/>
+    <hyperlink ref="G92" r:id="rId384" xr:uid="{00000000-0004-0000-0500-00008E010000}"/>
+    <hyperlink ref="H92" r:id="rId385" xr:uid="{00000000-0004-0000-0500-00008F010000}"/>
+    <hyperlink ref="I92" r:id="rId386" xr:uid="{00000000-0004-0000-0500-000090010000}"/>
+    <hyperlink ref="P92" r:id="rId387" xr:uid="{00000000-0004-0000-0500-000091010000}"/>
+    <hyperlink ref="R92" r:id="rId388" display="Referrals are an especially powerful tool for growing a startup. Unlike traditional forms of marketing, referrals are backed by trust and personal endorsements. This type of marketing not only spreads awareness of your business but also enhances its credibility." xr:uid="{00000000-0004-0000-0500-000092010000}"/>
+    <hyperlink ref="T92" r:id="rId389" xr:uid="{00000000-0004-0000-0500-000093010000}"/>
+    <hyperlink ref="U92" r:id="rId390" xr:uid="{00000000-0004-0000-0500-000094010000}"/>
+    <hyperlink ref="G93" r:id="rId391" xr:uid="{00000000-0004-0000-0500-000095010000}"/>
+    <hyperlink ref="H93" r:id="rId392" xr:uid="{00000000-0004-0000-0500-000096010000}"/>
+    <hyperlink ref="I93" r:id="rId393" xr:uid="{00000000-0004-0000-0500-000097010000}"/>
+    <hyperlink ref="P93" r:id="rId394" xr:uid="{00000000-0004-0000-0500-000098010000}"/>
+    <hyperlink ref="R93" r:id="rId395" display="&quot;Referral Power - Referrals backed by trust and personal endorsements spread awareness while enhancing credibility, unlike traditional marketing&quot;" xr:uid="{00000000-0004-0000-0500-000099010000}"/>
+    <hyperlink ref="G94" r:id="rId396" xr:uid="{00000000-0004-0000-0500-00009A010000}"/>
+    <hyperlink ref="H94" r:id="rId397" xr:uid="{00000000-0004-0000-0500-00009B010000}"/>
+    <hyperlink ref="I94" r:id="rId398" xr:uid="{00000000-0004-0000-0500-00009C010000}"/>
+    <hyperlink ref="P94" r:id="rId399" xr:uid="{00000000-0004-0000-0500-00009D010000}"/>
+    <hyperlink ref="R94" r:id="rId400" display="&quot;Competitive Reality - Assume competitors already exist; your product may not be as unique as you think. Differentiation requires deliberate strategy&quot;" xr:uid="{00000000-0004-0000-0500-00009E010000}"/>
+    <hyperlink ref="G95" r:id="rId401" xr:uid="{00000000-0004-0000-0500-00009F010000}"/>
+    <hyperlink ref="H95" r:id="rId402" location="the-best-marketing-frameworks" xr:uid="{00000000-0004-0000-0500-0000A0010000}"/>
+    <hyperlink ref="I95" r:id="rId403" xr:uid="{00000000-0004-0000-0500-0000A1010000}"/>
+    <hyperlink ref="P95" r:id="rId404" xr:uid="{00000000-0004-0000-0500-0000A2010000}"/>
+    <hyperlink ref="R95" r:id="rId405" display="&quot;Single-Channel Risk - Putting all growth efforts in one channel basket creates vulnerability; channel diversification is essential for scaling&quot;" xr:uid="{00000000-0004-0000-0500-0000A3010000}"/>
+    <hyperlink ref="P96" r:id="rId406" xr:uid="{00000000-0004-0000-0500-0000A4010000}"/>
+    <hyperlink ref="R96" r:id="rId407" xr:uid="{00000000-0004-0000-0500-0000A5010000}"/>
+    <hyperlink ref="T96" r:id="rId408" xr:uid="{00000000-0004-0000-0500-0000A6010000}"/>
+    <hyperlink ref="P97" r:id="rId409" xr:uid="{00000000-0004-0000-0500-0000A7010000}"/>
+    <hyperlink ref="R97" r:id="rId410" xr:uid="{00000000-0004-0000-0500-0000A8010000}"/>
+    <hyperlink ref="T97" r:id="rId411" xr:uid="{00000000-0004-0000-0500-0000A9010000}"/>
+    <hyperlink ref="P98" r:id="rId412" xr:uid="{00000000-0004-0000-0500-0000AA010000}"/>
+    <hyperlink ref="R98" r:id="rId413" xr:uid="{00000000-0004-0000-0500-0000AB010000}"/>
+    <hyperlink ref="P99" r:id="rId414" xr:uid="{00000000-0004-0000-0500-0000AC010000}"/>
+    <hyperlink ref="P100" r:id="rId415" xr:uid="{00000000-0004-0000-0500-0000AD010000}"/>
+    <hyperlink ref="R100" r:id="rId416" xr:uid="{00000000-0004-0000-0500-0000AE010000}"/>
+    <hyperlink ref="T100" r:id="rId417" xr:uid="{00000000-0004-0000-0500-0000AF010000}"/>
+    <hyperlink ref="P101" r:id="rId418" xr:uid="{00000000-0004-0000-0500-0000B0010000}"/>
+    <hyperlink ref="R101" r:id="rId419" xr:uid="{00000000-0004-0000-0500-0000B1010000}"/>
+    <hyperlink ref="T101" r:id="rId420" xr:uid="{00000000-0004-0000-0500-0000B2010000}"/>
+    <hyperlink ref="P102" r:id="rId421" xr:uid="{00000000-0004-0000-0500-0000B3010000}"/>
+    <hyperlink ref="R102" r:id="rId422" xr:uid="{00000000-0004-0000-0500-0000B4010000}"/>
+    <hyperlink ref="T102" r:id="rId423" xr:uid="{00000000-0004-0000-0500-0000B5010000}"/>
+    <hyperlink ref="U102" r:id="rId424" xr:uid="{00000000-0004-0000-0500-0000B6010000}"/>
+    <hyperlink ref="P103" r:id="rId425" xr:uid="{00000000-0004-0000-0500-0000B7010000}"/>
+    <hyperlink ref="R103" r:id="rId426" xr:uid="{00000000-0004-0000-0500-0000B8010000}"/>
+    <hyperlink ref="T103" r:id="rId427" xr:uid="{00000000-0004-0000-0500-0000B9010000}"/>
+    <hyperlink ref="U103" r:id="rId428" xr:uid="{00000000-0004-0000-0500-0000BA010000}"/>
+    <hyperlink ref="O104" r:id="rId429" xr:uid="{00000000-0004-0000-0500-0000BB010000}"/>
+    <hyperlink ref="P104" r:id="rId430" xr:uid="{00000000-0004-0000-0500-0000BC010000}"/>
+    <hyperlink ref="R104" r:id="rId431" display="Long-term goals are often overlooked in startups for reasons (or excuses) of agility but if you want to move fast, you need to know where you are going. You have to be able to make quick but smart decisions. And this requires a clear sense of direction." xr:uid="{00000000-0004-0000-0500-0000BD010000}"/>
+    <hyperlink ref="S104" r:id="rId432" xr:uid="{00000000-0004-0000-0500-0000BE010000}"/>
+    <hyperlink ref="T104" r:id="rId433" display="some startups rely too heavily on their original team members, who, despite being capable of managing early-stage growth, may lack the necessary skills and experience for later stages. That dependence can hold back a startup’s development and prevent it from achieving its full potential. Startups need to strike a balance between leveraging fresh perspectives with the insights of existing employees." xr:uid="{00000000-0004-0000-0500-0000BF010000}"/>
+    <hyperlink ref="U104" r:id="rId434" xr:uid="{00000000-0004-0000-0500-0000C0010000}"/>
+    <hyperlink ref="P105" r:id="rId435" xr:uid="{00000000-0004-0000-0500-0000C1010000}"/>
+    <hyperlink ref="R105" r:id="rId436" xr:uid="{00000000-0004-0000-0500-0000C2010000}"/>
+    <hyperlink ref="S105" r:id="rId437" xr:uid="{00000000-0004-0000-0500-0000C3010000}"/>
+    <hyperlink ref="T105" r:id="rId438" xr:uid="{00000000-0004-0000-0500-0000C4010000}"/>
+    <hyperlink ref="U105" r:id="rId439" xr:uid="{00000000-0004-0000-0500-0000C5010000}"/>
+    <hyperlink ref="P106" r:id="rId440" xr:uid="{00000000-0004-0000-0500-0000C6010000}"/>
+    <hyperlink ref="R106" r:id="rId441" xr:uid="{00000000-0004-0000-0500-0000C7010000}"/>
+    <hyperlink ref="T106" r:id="rId442" display="Encourage an environment of transparency, constructive feedback, and empathy among your team. Implementing feedback surveys (and listening to the feedback) or setting up times for team members to communicate and discuss their disagreements is essential for resolving conflicts. " xr:uid="{00000000-0004-0000-0500-0000C8010000}"/>
+    <hyperlink ref="U106" r:id="rId443" xr:uid="{00000000-0004-0000-0500-0000C9010000}"/>
+    <hyperlink ref="P107" r:id="rId444" xr:uid="{00000000-0004-0000-0500-0000CA010000}"/>
+    <hyperlink ref="R107" r:id="rId445" xr:uid="{00000000-0004-0000-0500-0000CB010000}"/>
+    <hyperlink ref="T107" r:id="rId446" xr:uid="{00000000-0004-0000-0500-0000CC010000}"/>
+    <hyperlink ref="U107" r:id="rId447" xr:uid="{00000000-0004-0000-0500-0000CD010000}"/>
+    <hyperlink ref="P108" r:id="rId448" xr:uid="{00000000-0004-0000-0500-0000CE010000}"/>
+    <hyperlink ref="R108" r:id="rId449" xr:uid="{00000000-0004-0000-0500-0000CF010000}"/>
+    <hyperlink ref="P109" r:id="rId450" xr:uid="{00000000-0004-0000-0500-0000D0010000}"/>
+    <hyperlink ref="R109" r:id="rId451" xr:uid="{00000000-0004-0000-0500-0000D1010000}"/>
+    <hyperlink ref="P110" r:id="rId452" xr:uid="{00000000-0004-0000-0500-0000D2010000}"/>
+    <hyperlink ref="R110" r:id="rId453" xr:uid="{00000000-0004-0000-0500-0000D3010000}"/>
+    <hyperlink ref="P111" r:id="rId454" xr:uid="{00000000-0004-0000-0500-0000D4010000}"/>
+    <hyperlink ref="R111" r:id="rId455" xr:uid="{00000000-0004-0000-0500-0000D5010000}"/>
+    <hyperlink ref="P112" r:id="rId456" xr:uid="{00000000-0004-0000-0500-0000D6010000}"/>
+    <hyperlink ref="R112" r:id="rId457" xr:uid="{00000000-0004-0000-0500-0000D7010000}"/>
+    <hyperlink ref="S112" r:id="rId458" xr:uid="{00000000-0004-0000-0500-0000D8010000}"/>
+    <hyperlink ref="P113" r:id="rId459" xr:uid="{00000000-0004-0000-0500-0000D9010000}"/>
+    <hyperlink ref="I10" r:id="rId460" xr:uid="{DC1CC40C-76BF-4151-B4AE-6B27A4A2CA83}"/>
+    <hyperlink ref="L17" r:id="rId461" xr:uid="{86177E8A-8D81-4E6A-9857-7126C272F5F9}"/>
+    <hyperlink ref="K18" r:id="rId462" xr:uid="{90524FBC-4648-460B-AF07-40CF07362549}"/>
+    <hyperlink ref="L18" r:id="rId463" xr:uid="{45C73B90-FD7A-47AC-8435-288C2341EA2C}"/>
+    <hyperlink ref="L24" r:id="rId464" xr:uid="{841EE744-F15D-4AD1-B723-3561AEDAD835}"/>
+    <hyperlink ref="L25" r:id="rId465" xr:uid="{06FA8D96-68AE-46E7-A79A-4A8DC12AD08C}"/>
+    <hyperlink ref="I28" r:id="rId466" display="PESTLE analysis" xr:uid="{0D490440-4354-4655-A3DD-EE81F7C6055A}"/>
+    <hyperlink ref="K39" r:id="rId467" xr:uid="{2ACB092F-8BB8-4B6E-9A08-8A35F74EE22A}"/>
+    <hyperlink ref="L39" r:id="rId468" xr:uid="{B625F6C3-BACC-46E9-88C0-E746813555A7}"/>
+    <hyperlink ref="K41" r:id="rId469" xr:uid="{3741B1DB-8273-4F29-B54C-88D8A0435455}"/>
+    <hyperlink ref="L41" r:id="rId470" xr:uid="{BA1B52BE-9404-49FC-A335-ED0787CA4FAA}"/>
+    <hyperlink ref="K43" r:id="rId471" location=":~:text=The%20Double%20Diamond%20is%20a,%E2%80%94%20solutions%20that%20work%20(converging)" xr:uid="{8B1BF22B-2F01-4A9F-8BAC-3F87FC74ACB7}"/>
+    <hyperlink ref="K44" r:id="rId472" location=":~:text=They%20focus%20on%20people%20and,Finally%2C%20they%20do%20small%20interventions." xr:uid="{F923DCE5-903C-4C42-B606-F89F10046C40}"/>
+    <hyperlink ref="H5" r:id="rId473" xr:uid="{BE6E9774-A880-45F8-8ED1-2C6482C46851}"/>
+    <hyperlink ref="G5" r:id="rId474" xr:uid="{2C4CBDFB-296B-4ADF-A1BE-EE19D2A7F865}"/>
+    <hyperlink ref="J7" r:id="rId475" xr:uid="{92D8F356-A1FF-4F87-B03D-C34C7A09C64E}"/>
+    <hyperlink ref="K7" r:id="rId476" xr:uid="{6825C89D-5444-4995-9806-D6E89DD5CBE7}"/>
+    <hyperlink ref="H9" r:id="rId477" xr:uid="{9A76F0FB-C178-46D3-A7D8-9024FAAF9D97}"/>
+    <hyperlink ref="G9" r:id="rId478" xr:uid="{630C9616-0E5C-4651-A337-654125678644}"/>
+    <hyperlink ref="J10" r:id="rId479" xr:uid="{3C841678-6F8C-4428-90E6-C893A557463E}"/>
+    <hyperlink ref="H10" r:id="rId480" xr:uid="{132EBC56-BDE1-4359-B18E-6DA3FD5113BF}"/>
+    <hyperlink ref="I31" r:id="rId481" xr:uid="{00000000-0004-0000-0500-000083000000}"/>
+    <hyperlink ref="T32" r:id="rId482" xr:uid="{CAD8C31C-98EF-4F8F-A865-FB61F17AA62A}"/>
+    <hyperlink ref="R32" r:id="rId483" xr:uid="{B6BA9457-7FC4-4838-B63A-C209AFC28F78}"/>
+    <hyperlink ref="H57" r:id="rId484" display="PESTLE analysis" xr:uid="{706B041A-8422-4768-8FF3-DB11748C24A7}"/>
+    <hyperlink ref="N61" r:id="rId485" xr:uid="{03235505-13B9-4900-8D97-98A45CC7E9CE}"/>
+    <hyperlink ref="R61" r:id="rId486" display="To expect communication naturally evolves with growth, for instance, is a false assumption many startup founders make. It’s obviously a lot easier to communicate changes and progress to a few other people, versus 10, 50 or even 1000 other people." xr:uid="{F719F4D6-E9DA-44FB-BA73-3F801A64E73B}"/>
+    <hyperlink ref="H90" r:id="rId487" xr:uid="{C8DC8E67-047A-42D9-99A3-7989946866BB}"/>
+    <hyperlink ref="G10" r:id="rId488" xr:uid="{6B4FE341-660E-4816-8C8E-F3E6F606E3AF}"/>
+    <hyperlink ref="G6" r:id="rId489" xr:uid="{9CFCAFB9-3246-4720-941D-AC16CBC47BC8}"/>
+    <hyperlink ref="K9" r:id="rId490" display="Jobs To Be Done Framework" xr:uid="{5D955235-3777-417A-83C7-9F8C7EE7F5B3}"/>
+    <hyperlink ref="J8" r:id="rId491" display="Pilot Program Framework" xr:uid="{49F44223-C389-4AC9-9EC1-20DEAF774550}"/>
+    <hyperlink ref="K10" r:id="rId492" xr:uid="{86063A33-ACBC-4811-B4E1-83A5DA720088}"/>
+    <hyperlink ref="G2" r:id="rId493" xr:uid="{586CE265-4B41-4F55-BD8E-52C453AE3422}"/>
+    <hyperlink ref="F54" r:id="rId494" xr:uid="{DD31E9B4-7FA1-407A-9E7D-7F39E84FB5CE}"/>
+    <hyperlink ref="G54" r:id="rId495" xr:uid="{07F9CEF7-E310-49A0-A8F9-99CF4F2FF981}"/>
+    <hyperlink ref="H28" r:id="rId496" xr:uid="{20F27F8A-811A-4DCD-8294-51381FA3779A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId497"/>

</xml_diff>

<commit_message>
v6.52: Final session update - Excel links + documentation
- Regenerated questions-data.js from Self Assessment Structure - Master.xlsx
- 113 questions, 496 hyperlinks with updated Resources/Tools links
- Updated CLAUDE.md with full session history
- Version history: v6.44 through v6.51

Session fixes included:
- Mobile prelim layout (space-between alignment)
- Start Fresh button right-alignment
- Pull-to-refresh restored
- Different How It Works guidance per path
- Validation info buttons right-aligned
- Sova Quick Start DOCX colours updated

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Self Assessment Structure - Master.xlsx
+++ b/Self Assessment Structure - Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\janek\sova-mvp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2FDDEB-4C52-4A28-B414-B28D0DDD9CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABD0668-71C4-4FF1-8D02-10DBD0E852A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5690,12 +5690,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6253,7 +6253,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>1348</v>
       </c>
       <c r="B2" s="34"/>
@@ -6373,7 +6373,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="33" t="s">
         <v>1375</v>
       </c>
       <c r="B11" s="34"/>
@@ -6479,7 +6479,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="33" t="s">
         <v>1404</v>
       </c>
       <c r="B19" s="34"/>
@@ -6571,7 +6571,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="33" t="s">
         <v>1429</v>
       </c>
       <c r="B26" s="34"/>
@@ -6775,7 +6775,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="33" t="s">
         <v>1486</v>
       </c>
       <c r="B41" s="34"/>
@@ -6853,7 +6853,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="33" t="s">
         <v>1507</v>
       </c>
       <c r="B47" s="34"/>
@@ -7113,7 +7113,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="33" t="s">
         <v>1578</v>
       </c>
       <c r="B66" s="34"/>
@@ -7121,7 +7121,7 @@
       <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="33" t="s">
+      <c r="A67" s="35" t="s">
         <v>1579</v>
       </c>
       <c r="B67" s="34"/>
@@ -7227,7 +7227,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="35" t="s">
         <v>1607</v>
       </c>
       <c r="B75" s="34"/>
@@ -7277,7 +7277,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" s="33" t="s">
+      <c r="A79" s="35" t="s">
         <v>1620</v>
       </c>
       <c r="B79" s="34"/>
@@ -7299,7 +7299,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="35" t="s">
         <v>1625</v>
       </c>
       <c r="B81" s="34"/>
@@ -7321,7 +7321,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="33" t="s">
+      <c r="A83" s="35" t="s">
         <v>1630</v>
       </c>
       <c r="B83" s="34"/>
@@ -7358,11 +7358,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A66:D66"/>
     <mergeCell ref="A75:D75"/>
     <mergeCell ref="A67:D67"/>
     <mergeCell ref="A79:D79"/>
@@ -7370,6 +7365,11 @@
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7946,10 +7946,10 @@
   <dimension ref="A1:U117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>